<commit_message>
Commited with data clean up
</commit_message>
<xml_diff>
--- a/Team02_NinjaScrapers_2023/src/test/resources/AllergyRecipes.xlsx
+++ b/Team02_NinjaScrapers_2023/src/test/resources/AllergyRecipes.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{69DBBAC3-E6FD-4D82-B715-EEB8DF14CC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akash\git\RecipeScrapingHackathon2023\Team02_NinjaScrapers_2023\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546B0DCE-F65E-47D1-BB3F-4A5895534C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,12 +16,11 @@
     <sheet name="AllergyToAdd" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="827">
   <si>
     <t>Recipe ID</t>
   </si>
@@ -2830,12 +2834,2304 @@
   <si>
     <t>https://www.tarladalal.com/how-to-soak-garden-cress-seeds-42833r</t>
   </si>
+  <si>
+    <t xml:space="preserve"> 3883</t>
+  </si>
+  <si>
+    <t>Masala Chawli</t>
+  </si>
+  <si>
+    <t>Healthy Sabzis with Gravies</t>
+  </si>
+  <si>
+    <t>For Masala Chawli
+1/2 cup chawli (cow pea / lobhia) , soaked overnight and drained
+salt to taste
+1 tbsp coconut oil or oil
+1/2 cup finely chopped onions
+1 cup fresh tomato pulp
+1/2 tsp dried fenugreek leaves (kasuri methi)
+1/4 tsp turmeric powder (haldi)
+To Be Ground Into A Smooth Mint Paste
+3/4 cup chopped mint leaves (phudina) , washed and drained
+1 tsp roughly chopped ginger (adrak)
+2 tsp roughly chopped green chillies
+1/2 tsp lemon juice</t>
+  </si>
+  <si>
+    <t>23 mins</t>
+  </si>
+  <si>
+    <t>Method
+For masala chawli
+To make masala chawli, first prepare the mint paste by putting in a mixer, mint leaves, ginger, green chillies, lemon juice and 2 tbsp water. Grind to a smooth paste.
+Combine the soaked chawli, salt and 1 cup of water in a pressure cooker, mix well and pressure cook for 2 whistles.
+Allow the steam to escape before opening the lid. Do not discard the water. Keep aside.
+Heat the coconut oil or oil in a deep non-stick pan, add the onions and sauté on a medium flame for 1 to 2 minutes.
+Add the fresh tomato pulp, the dried fenugreek leaves, turmeric powder, a little salt, cooked chawli along with the water, mint paste and mix well.
+Cook on a medium flame for 4 to 5 minutes, while stirring occasionally.
+Serve masala chawli hot with bajra roti or roti.</t>
+  </si>
+  <si>
+    <t>Energy 122 cal
+Protein 5.8 g
+Carbohydrates 15.2 g
+Fiber 4.6 g
+Fat 4.1 g
+Cholesterol 0 mg
+Sodium 12.9 mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hypothyroidism Recipes
+</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/masala-chawli-3883r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3577</t>
+  </si>
+  <si>
+    <t>Turai Aur Moong ki Dal</t>
+  </si>
+  <si>
+    <t>Pressure Cooker</t>
+  </si>
+  <si>
+    <t>1/4 cup yellow moong dal (split yellow gram)
+2 cups peeled and chopped ridge gourd (turai)
+1/4 cup finely chopped onions
+1 tsp ginger-green chilli paste
+1/4 tsp turmeric powder (haldi)
+1/4 tsp cumin seeds (jeera)
+a pinch of asafoetida (hing)
+1 tsp chilli powder
+1/4 tsp garam masala
+1 tsp oil
+salt to taste
+For the garnish
+2 tbsp chopped coriander (dhania)</t>
+  </si>
+  <si>
+    <t>15 mins.</t>
+  </si>
+  <si>
+    <t>20 mins.</t>
+  </si>
+  <si>
+    <t>Method
+Clean and wash the moong dal.
+Combine the moong dal, turai, onion, ginger-green chilli paste and turmeric powder with 2 cups of water and pressure cook for 2 to 3 whistles or until the dal is cooked.
+For the tempering, heat the oil in a non-stick pan, add the cumin seeds, asafoetida, chilli powder and garam masala and fry till the seeds crackle.
+Pour this tempering over the prepared dal. Add salt and simmer for 5 to 7 minutes.
+Serve hot, garnished with the coriander.</t>
+  </si>
+  <si>
+    <t>Energy 56 cal
+Protein 2.6 g
+Carbohydrates 8.1 g
+Fiber 1.6 g
+Fat 1.4 g
+Cholesterol 0 mg
+Sodium 4.2 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/turai-aur-moong-ki-dal-3577r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 38470</t>
+  </si>
+  <si>
+    <t>Chana, Tuvar and Green Moong Dal, Trevati Dal</t>
+  </si>
+  <si>
+    <t>Pan</t>
+  </si>
+  <si>
+    <t>For Chana , Tuvar and Green Moong Dal
+1/2 cup chana dal (split bengal gram)
+1/2 cup toovar (arhar) dal
+1/2 cup green moong dal (split green gram)
+1 tsp cumin seeds (jeera)
+2 cloves (laung / lavang)
+2 bay leaves (tejpatta)
+2 whole dry kashmiri red chillies
+1/4 tsp asafoetida (hing)
+1/2 cup finely chopped onions
+2 tsp finely chopped green chillies
+2 tbsp finely chopped garlic (lehsun)
+1 tsp chopped ginger (adrak)
+1/2 cup chopped tomatoes
+1 tsp chilli powder
+1/4 tsp turmeric powder (haldi)
+1 tbsp lemon juice
+2 tbsp oil
+salt to taste
+For The Garnish
+2 tbsp finely chopped coriander (dhania)</t>
+  </si>
+  <si>
+    <t>Method
+For chana, tuvar and green moong dal
+To make chana, tuvar and green moong dal, clean, wash and soak the dals in water about 30 minutes. Drain.
+Combine the soaked dals, salt and 3½ cups of water in a pressure cooker and pressure cook for 2 whistles.
+Allow the steam to escape before opening the lid. Keep aside.
+Heat the oil in a pan, add the cumin seeds, cloves, bayleaves, red chillies and asafoetida and sauté on a medium flame for a few seconds.
+Add the onions, green chillies, garlic and ginger and sauté on a medium flame for 1 to 2 minutes.
+Add the tomatoes, chilli powder and turmeric powder, mix well and cook on a medium flame for 3 to 4 minutes or till the oil separates from the masala.
+Add the dals and 2 cups of water, lemon juice and salt and simmer for 10 minutes.
+Serve the chana, tuvar and green moong dal hot garnished with the chopped coriander.
+Handy tip :
+To make a "jain" trevati dal, omit the onions, ginger and garlic and proceed as per the recipe.</t>
+  </si>
+  <si>
+    <t>Energy 229 cal
+Protein 11.4 g
+Carbohydrates 31.3 g
+Fiber 5.7 g
+Fat 6.5 g
+Cholesterol 0 mg
+Sodium 23.4 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/chana-tuvar-and-green-moong-dal-trevati-dal-38470r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22229</t>
+  </si>
+  <si>
+    <t>Hearty Red Lentil Soup, Healthy Masoor Dal Soup</t>
+  </si>
+  <si>
+    <t>Home Remedies Protein Rich</t>
+  </si>
+  <si>
+    <t>For Red Lentil Soup
+1/2 cup masoor (split red lentil) dal , washed and drained
+1/4 cup finely chopped mint leaves (phudina)
+3/4 cup roughly chopped onions
+3/4 cup roughly chopped carrot
+1/4 cup roughly chopped tomatoes
+1/2 tsp dry red chilli flakes (paprika)
+salt to taste</t>
+  </si>
+  <si>
+    <t>Method
+Heat a small non-stick pan and when hot, add the mint leaves and dry roast on a slow flame for 3 minutes. Keep aside.
+Combine the masoor dal, onions, carrot, tomatoes and 2 cups of water in a pressure cooker, mix well and pressure cook for 2 whistles.
+Allow the steam to escape before opening the lid.
+Cool slightly and blend in a mixer till smooth.
+Transfer the mixture into a deep non-stick pan, add the roasted mint leaves, chilli flakes, salt, 1 cup of water and mix well and cook on a medium flame for 3 to 4 minutes, while stirring occasionally.
+Serve hot.</t>
+  </si>
+  <si>
+    <t>Energy 94 cal
+Protein 5.5 g
+Carbohydrates 17.5 g
+Fiber 3.7 g
+Fat 0.2 g
+Cholesterol 0 mg
+Sodium 13.9 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/hearty-red-lentil-soup-healthy-masoor-dal-soup-22229r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 40603</t>
+  </si>
+  <si>
+    <t>Baingan Bhaja, Bengali Begun Bhaja</t>
+  </si>
+  <si>
+    <t>For Baingan Bhaja
+18 big brinjal (baingan / eggplant) slices
+2 tsp chilli powder
+1/2 tsp turmeric powder (haldi)
+1 tbsp lemon juice
+1/4 cup besan (bengal gram flour)
+salt to taste
+2 tsp oil for greasing and cooking</t>
+  </si>
+  <si>
+    <t>Method
+For baingan bhaja
+To make baingan bhaja, combine the chilli powder, turmeric powder, lemon juice, besan, salt and 2 tbsp of water in a deep bowl and mix well.
+Add the baingan slices and mix well. Keep aside.
+Heat a non-stick tava (griddle), grease it with ½ tsp of oil, arrange half the baingan slices and cook using ½ tsp of oil on both the sides till golden brown in colour.
+Repeat step 3 to make 1 more batch.
+Serve the baingan bhaja immediately.</t>
+  </si>
+  <si>
+    <t>Energy 43 cal
+Protein 1.5 g
+Carbohydrates 4.6 g
+Fiber 3 g
+Fat 2.1 g
+Cholesterol 0 mg
+Sodium 4.3 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/baingan-bhaja-bengali-begun-bhaja-40603r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5292</t>
+  </si>
+  <si>
+    <t>Dal Moghlai ( Low Cholesterol Recipe)</t>
+  </si>
+  <si>
+    <t>Indian Party</t>
+  </si>
+  <si>
+    <t>For Dal Moghlai
+3/4 cup toovar (arhar) dal
+1/4 cup chana dal (split bengal gram)
+1 cup chopped tomatoes
+2 cups bottle gourd (doodhi / lauki) , cut into big pieces
+1/4 tsp turmeric powder (haldi)
+1 tsp cumin seeds (jeera)
+1/2 tsp chopped garlic (lehsun)
+1 tsp chopped green chillies
+1 tsp grated ginger (adrak)
+3/4 cup sliced onions
+2 tsp oil
+salt to taste
+For The Garnish
+2 tbsp chopped coriander (dhania)</t>
+  </si>
+  <si>
+    <t>Method
+For dal moghlai
+To make dal moghlai,clean, wash and soak the dals for about 30 minutes. Drain.
+Add the tomatoes, bottle gourd, turmeric powder, salt and 3 cups of water and pressure cook till the dals are tender.
+Heat the oil in a large non-stick pan and add the cumin seeds.
+When the seeds crackle, add the garlic, green chillies, ginger and onions and sauté till the onions turn golden brown in colour. Sprinkle about 1 tablespoon of water over it to prevent the onions from burning.
+Add the cooked dal mixture and 1 cup of water and bring to boil.
+Serve dal moghlai hot garnished with coriander.</t>
+  </si>
+  <si>
+    <t>Energy 130 cal
+Protein 6.7 g
+Carbohydrates 19.8 g
+Fiber 4.6 g
+Fat 2.6 g
+Cholesterol 0 mg
+Sodium 16.5 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/dal-moghlai--low-cholesterol-recipe-5292r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 35288</t>
+  </si>
+  <si>
+    <t>Oats Moong Dal Tikki</t>
+  </si>
+  <si>
+    <t>For Oats Moong Dal Tikki
+1/2 cup yellow moong dal (split yellow gram)
+1/2 cup quick cooking rolled oats
+2 tbsp fresh curd (dahi)
+3 tbsp grated onions
+1/2 tsp finely chopped green chillies
+2 tsp chaat masala
+2 tsp chilli powder
+1/4 tsp garam masala
+1/4 tsp turmeric powder (haldi)
+1 tsp ginger-garlic (adrak-lehsun) paste
+2 tbsp finely chopped coriander (dhania)
+salt to taste
+2 tsp oil for greasing and cooking
+For Serving With Oats Moong Dal Tikki
+healthy green chutney</t>
+  </si>
+  <si>
+    <t>Method
+For oats moong dal tikki
+To make oats moong dal tikki, clean, wash and boil the yellow moong dal in 1 cup of water in a deep pan till the dal is soft and cooked and all the water has evaporated.
+Drain and blend the dal in a mixer to a coarse paste.
+Transfer the paste into a bowl, add all the remaining ingredients and mix well.
+Divide the mixture into 12 equal portions and shape each portion into a 63 mm. (2½”) round flat tikki.
+Lightly grease a non-stick tava (griddle) with ½ tsp of oil.
+Cook each oats moong dal tikki, using 1/8 tsp of oil, till they turn golden brown in colour from both the sides. Evenly cooked from both the sides.
+Serve the oats moong dal tikki immediately with healthy green chutney.</t>
+  </si>
+  <si>
+    <t>Energy 54 cal
+Protein 2.7 g
+Carbohydrates 7.7 g
+Fiber 1.1 g
+Fat 1.3 g
+Cholesterol 0.4 mg
+Sodium 3.2 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/oats-moong-dal-tikki-35288r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 36424</t>
+  </si>
+  <si>
+    <t>Buckwheat Dosa</t>
+  </si>
+  <si>
+    <t>Mixer</t>
+  </si>
+  <si>
+    <t>For Buckwheat Dosas
+1 cup buckwheat (kuttu or kutti no daro)
+1/4 cup urad dal (split black lentils)
+1 tbsp oil
+1 tsp mustard seeds ( rai / sarson)
+1/4 tsp asafoetida (hing)
+2 tsp finely chopped green chillies
+2 tbsp finely chopped coriander (dhania)
+salt to taste
+Other Ingredients For Buckwheat Dosas
+oil for greasing and cooking
+For Serving With Buckwheat Dosas
+green chutney</t>
+  </si>
+  <si>
+    <t>Method
+For buckwheat dosas
+To make buckwheat dosas, combine the buckwheat and urad dal in a mixer and blend to a fine powder.
+Transfer the powder in a deep bowl and keep aside.
+Heat the oil in a small pan and add the mustard seeds.
+When the seeds crackle, add the asafoetida and sauté on a medium flame for a few seconds.
+Add the tempering, green chillies, coriander, salt and approximately 3 ¼ cups of water and mix well.
+Heat a non-stick tava (griddle) and grease it lightly with oil.
+Pour a ladleful of batter in a circular manner. Pour a little oil in the holes of the buckwheat dosa and cook on both the sides till golden brown in colour.
+Repeat step 7 to make 19 more buckwheat dosas.
+Serve the buckwheat dosas immediately with green chutney.</t>
+  </si>
+  <si>
+    <t>Energy 45 cal
+Protein 1.4 g
+Carbohydrates 6.1 g
+Fiber 0.9 g
+Fat 1.7 g
+Cholesterol 0 mg
+Sodium 2.3 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/buckwheat-dosa-36424r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 42296</t>
+  </si>
+  <si>
+    <t>Quinoa Avocado Veg Healthy Office Salad</t>
+  </si>
+  <si>
+    <t>High Fiber Indian Salads</t>
+  </si>
+  <si>
+    <t>1/4 cup cooked quinoa
+1/2 cup riped avocado cubes
+1/2 cup chopped zucchini
+1/2 cup coloured capsicum cubes
+1/4 cup mushroom (khumbh) cubes
+1/4 cup cherry tomato halves
+1 cup iceberg lettuce , torn into pieces
+1 tbsp alfalfa sprouts
+1 tsp olive oil
+sea salt (khada namak) to taste
+To Be Mixed Into A Dressing
+1 tbsp olive oil
+1 tsp lemon juice
+1/4 tsp grated garlic (lehsun)
+sea salt (khada namak) to taste</t>
+  </si>
+  <si>
+    <t>3 mins</t>
+  </si>
+  <si>
+    <t>Method
+Heat the olive oil in a griller pan or a broad non-stick pan, add the zucchini and sauté on a medium flame for 1 minute.
+Add the coloured capsicum and sauté on a medium flame for 1 minute.
+Add the mushroom and little sea salt and sauté on a medium flame for 1 minute.
+Cool put in a lunch box, along with other ingredients. It can be taken to work with a dressing in a separate small container.
+Just before eating, mix the dressing and toss well. Eat immediately.</t>
+  </si>
+  <si>
+    <t>Energy 459 cal
+Protein 7.7 g
+Carbohydrates 22 g
+Fiber 6.9 g
+Fat 38.9 g
+Cholesterol 0 mg
+Sodium 60.1 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/quinoa-avocado-veg-healthy-office-salad-42296r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 39929</t>
+  </si>
+  <si>
+    <t>Brown Rice ( Pressure Cooker Method)</t>
+  </si>
+  <si>
+    <t>Biryani Recipes for Indian Dinner, Rice Pulao</t>
+  </si>
+  <si>
+    <t>For Brown Rice
+3/4 cup brown rice
+salt to taste</t>
+  </si>
+  <si>
+    <t>Method
+How to cook brown rice
+To cook brown rice, soak the brown rice in enough water for 30 minutes and drain well.
+Combine the brown rice along with 2 cups of water in a pressure cooker and pressure cook for 7 whistles.
+Allow the steam to escape before opening the lid.
+Separate each grain of the brown rice lightly with a fork. Use as required.</t>
+  </si>
+  <si>
+    <t>Energy 211 cal
+Protein 4.4 g
+Carbohydrates 44.4 g
+Fiber 2 g
+Fat 1.6 g
+Cholesterol 0 mg
+Sodium 2.3 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/brown-rice--pressure-cooker-method-39929r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6229</t>
+  </si>
+  <si>
+    <t>Beetroot Juice, Healthy Beetroot Juice</t>
+  </si>
+  <si>
+    <t>low cholesterol Indian drinks, juices</t>
+  </si>
+  <si>
+    <t>For Beetroot Juice
+1 1/2 cups beetroot cubes
+1 1/2 cups carrot cubes
+2 tbsp chopped parsley
+2 tbsp chopped celery (ajmoda)
+1/4 tsp black salt (sanchal)
+12 ice-cubes</t>
+  </si>
+  <si>
+    <t>Method
+Beetroot juice in blender
+Combine the beetroot cubes, carrots cubes, chopped parsley, chopped celery, black salt ( kala namak), 1 1/2 cups of water and 12 ice-cubes in a high quality blender jar (like vitamix) and blend well.
+Serve immediately.
+Mixer method
+This recipe doesn’t turn out good in a mixer jar because the texture of ingredients like carrots and beetroot are very hard.
+Handy tip:
+This recipe makes use of unpeeled fruits and vegetables, hence take care to clean and wash them well before chopping, to get rid of dirt, germs and chemical residues.</t>
+  </si>
+  <si>
+    <t>Energy 53 cal
+Protein 1.9 g
+Carbohydrates 11.1 g
+Fiber 4.5 g
+Fat 0.2 g
+Cholesterol 0 mg
+Sodium 69 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/beetroot-juice-healthy-beetroot-juice-6229r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 40586</t>
+  </si>
+  <si>
+    <t>Masoor Dal, Easy Masoor Dal Recipe</t>
+  </si>
+  <si>
+    <t>Pregnancy Hypothyroidism Diet</t>
+  </si>
+  <si>
+    <t>3/4 cup masoor dal (split red lentil) , washed and drained
+salt to taste
+1 tbsp oil
+1 tsp cumin seeds (jeera)
+1/4 tsp asafoetida (hing)
+1/2 cup finely chopped onions
+6 curry leaves (kadi patta)
+1 tsp garlic (lehsun) paste
+1 cup chopped tomatoes
+1 tsp chilli powder
+1 tsp coriander (dhania) powder
+1 tsp ginger-green chilli paste
+1/2 tsp turmeric powder (haldi)
+1/4 cup finely chopped coriander (dhania)</t>
+  </si>
+  <si>
+    <t>Method
+Combine the masoor dal, little salt and 2 cups of water in a pressure cooker and pressure cook for 2 whistles.
+Allow the steam to escape before opening the lid. Keep aside.
+Heat the ghee in a deep non-stick pan and add the cumin seeds and asafoetida and sauté on a medium flame for 30 seconds.
+Add the onions, curry leaves and garlic paste and sauté on a medium flame for 1 minute.
+Add the tomatoes, chilli powder, coriander powder, ginger-green chilli paste, turmeric powder and salt, mix well and cook on a medium flame for 2 minutes ,while stirring occasionally.
+Add the cooked masoor dal, 1 cup of water and coriander, mix well and cook on a medium flame for 4 minutes, while stirring occasionally.
+Serve hot.</t>
+  </si>
+  <si>
+    <t>Energy 148 cal
+Protein 7.8 g
+Carbohydrates 20.1 g
+Fiber 3.8 g
+Fat 4.1 g
+Cholesterol 0 mg
+Sodium 8.6 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/masoor-dal-easy-masoor-dal-recipe-40586r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 42333</t>
+  </si>
+  <si>
+    <t>Egg Paratha</t>
+  </si>
+  <si>
+    <t>Healthy Rotis Healthy Parathas Theplas</t>
+  </si>
+  <si>
+    <t>For The Parathas
+3/4 cup whole wheat flour (gehun ka atta)
+1/2 tsp carom seeds (ajwain)
+salt to taste
+whole wheat flour (gehun ka atta) for rolling
+1/2 tsp ghee for spreading
+1 tsp oil for cooking
+For The Egg Mixture
+3 eggs
+1/4 cup finely chopped onions
+1/4 cup finely chopped tomatoes
+2 tbsp finely chopped coriander (dhania)
+1 tsp finely chopped green chillies
+salt to taste
+Other Ingredients For Egg Paratha
+2 tsp oil for greasing
+2 tsp oil for cooking</t>
+  </si>
+  <si>
+    <t>Method
+For the parathas
+Combine all the ingredients in a deep bowl and knead into a soft dough using enough water.
+Divide the dough into 2 equal portions.
+Roll a portion of the dough into 150 mm. (6”) diameter circle using a little whole wheat flour for rolling. Spread ¼ tsp of ghee evenly over it.
+Fold over from one end to another end slightly overlapping each other.
+Then fold again from one end to another end overlapping each other.
+Roll again into a 175 mm. (7”) diameter circle using a little whole wheat flour for rolling.
+Heat a non-stick tava (griddle) and cook the paratha using ½ tsp of oil till it turns golden brown in colour from both the sides
+Repeat steps 3 to 7 to make 1 more paratha. Keep aside.
+For the egg mixture
+Break the eggs in a deep bowl and beat well using a fork.
+Add all the other ingredients and beat well. Keep aside.
+How to proceed
+To make egg paratha, heat a non-stick tava (griddle) and grease it using 1 tsp of oil. Pour half the egg mixture on it.
+Place a prepared paratha on it and press it lightly. Cook using 1 tsp of oil.
+Turnover and cook again till it is cooked.
+Cut into 4 equal portions using a cutter or a sharp knife.
+Repeat steps 1 to 4 to make 1 more egg paratha.
+Serve egg paratha immediately.</t>
+  </si>
+  <si>
+    <t>Energy 432 cal
+Protein 16.4 g
+Carbohydrates 38.3 g
+Fiber 6.5 g
+Fat 24.5 g
+Cholesterol 0 mg
+Sodium 14.7 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/egg-paratha-42333r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22378</t>
+  </si>
+  <si>
+    <t>Barley Moong Dal Vegetable Khichdi, Jau Dal Khichdi</t>
+  </si>
+  <si>
+    <t>Acidity Khichdi and Rice</t>
+  </si>
+  <si>
+    <t>For Barley Moong Dal Vegetable Khichdi
+1/2 cup barley (jau) , washed and drained
+3/4 cup yellow moong dal (split yellow gram) , washed and drained
+1 cup grated bottle gourd (doodhi / lauki)
+1 cup grated carrot
+1/2 tbsp ghee
+1 tsp cumin seeds (jeera)
+1/2 tsp asafoetida (hing)
+3 peppercorns (kalimirch)
+1 bay leaf (tejpatta)
+2 cloves (laung / lavang)
+1/2 tsp turmeric powder (haldi)
+salt to taste</t>
+  </si>
+  <si>
+    <t>Method
+For barley moong dal vegetable khichdi
+To make barley moong dal vegetable khichdi, heat the ghee in a pressure cooker and add the cumin seeds.
+When the seeds crackle, add the asafoetida, peppercorns, bayleaf and cloves and sauté on a medium flame for a few seconds.
+Add the bottle gourd and carrot and sauté on a medium flame for 1 minute.
+Add the barley, moong dal, turmeric powder, salt and 4½ cups of hot water, mix well and pressure cook for 3 whistles.
+Allow the steam to escape before opening the lid.
+Serve the barley moong dal vegetable khichdi immediately.</t>
+  </si>
+  <si>
+    <t>Energy 148 cal
+Protein 7.4 g
+Carbohydrates 25.8 g
+Fiber 3.6 g
+Fat 1.7 g
+Cholesterol 0 mg
+Sodium 14.1 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/barley-moong-dal-vegetable-khichdi-jau-dal-khichdi-22378r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22173</t>
+  </si>
+  <si>
+    <t>Khatta Urad Dal ( Zero Oil Urad Dal Recipe)</t>
+  </si>
+  <si>
+    <t>1 cup urad dal (split black lentils)
+1/2 cup whisked sour low-fat curds (dahi)
+1/2 tsp garlic (lehsun) paste
+1 tsp green chilli paste
+salt to taste
+1/2 tsp turmeric powder (haldi)
+2 tbsp chopped coriander (dhania)</t>
+  </si>
+  <si>
+    <t>22 mins</t>
+  </si>
+  <si>
+    <t>Method
+Clean, wash and soak the urad dal in enough water in a bowl for 15 minutes. Drain well.
+Combine the urad dal and 1½ cups of water in a pressure cooker, mix well and pressure cook for 3 whistles.
+Allow the steam to escape before opening the lid.
+Add the curds, 1½ cups of water, garlic paste, green chilli paste, salt and turmeric powder and mix well.
+Bring to boil and cook on a slow flame for 10 minutes, while stirring occasionally.
+Add the coriander and mix well.
+Serve hot.
+Handy tip:
+This dal tends to thicken if kept for too long. So, if you have made it in advance, add little water to it and re-heat it before serving.</t>
+  </si>
+  <si>
+    <t>Energy 192 cal
+Protein 13.5 g
+Carbohydrates 32.8 g
+Fiber 6.2 g
+Fat 0.8 g
+Cholesterol 0 mg
+Sodium 34.3 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/khatta-urad-dal--zero-oil-urad-dal-recipe-22173r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4829</t>
+  </si>
+  <si>
+    <t>Moong Dal Methi Sabzi</t>
+  </si>
+  <si>
+    <t>Strong Bones</t>
+  </si>
+  <si>
+    <t>For Moong Dal Methi Sabzi
+2 cups chopped fenugreek (methi) leaves
+1/4 cup yellow moong dal (split yellow gram)
+1/2 tsp cumin seeds (jeera)
+1/4 cup chopped onions
+1 tsp finely chopped garlic (lehsun)
+2 tsp finely chopped green chillies
+1/2 tsp turmeric powder (haldi)
+1 tsp oil
+salt to taste</t>
+  </si>
+  <si>
+    <t>Method
+For moong dal methi sabzi
+To make moong dal methi sabzi, wash and soak the yellow moong dal in enough water for 2 hours. Drain.
+Combine the soaked and drained moong dal and 5 tbsp of water in a deep pan, cover with a lid and cook on a medium flame for 6 to 8 minutes, while stirring occasionally. Keep aside.
+Heat the oil and add the cumin seeds.
+When they crackle, add the onions, garlic and green chillies and sauté for 1 minute.
+Add the fenugreek leaves, turmeric powder and salt and cook for 2 minutes.
+Add the soaked moong dal and 1 tbsp of water, mix well and cook on a medium flame for 1 minute.
+Serve moong dal methi sabzi hot with rotis.</t>
+  </si>
+  <si>
+    <t>Energy 106 cal
+Protein 5.6 g
+Carbohydrates 14 g
+Fiber 4.2 g
+Fat 3.1 g
+Cholesterol 0 mg
+Sodium 27.9 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/moong-dal-methi-sabzi-4829r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 42660</t>
+  </si>
+  <si>
+    <t>Baked Buckwheat Puri, Healthy Kuttu ki Puri</t>
+  </si>
+  <si>
+    <t>Evening Tea Snacks</t>
+  </si>
+  <si>
+    <t>For Baked Buckwheat Puri
+1/2 cup buckwheat (kuttu or kutti no daro) flour
+1/2 tsp olive oil
+1/2 tsp nigella seeds (kalonji)
+1/2 tsp green chilli paste
+1/4 tsp salt
+1/2 tsp olive oil for greasing
+buckwheat (kuttu or kutti no daro) flour for rolling</t>
+  </si>
+  <si>
+    <t>Method
+For baked buckwheat puri
+To make baked buckwheat puri, combine all the ingredients in a deep bowl and knead into a stiff dough using enough water.
+Divide the dough into 20 equal portions.
+Roll out each portion into a 50 mm. (2”) diameter circle using very little flour for rolling
+Arrange them on a greased baking tray and prick each puri with a fork at regular intervals.
+Bake in a pre-heated oven at 200°c (360°f) for 15 minutes.
+Cool the baked buckwheat puri slightly and serve or store in an air-tight container and use as required.</t>
+  </si>
+  <si>
+    <t>Energy 47 cal
+Protein 1.5 g
+Carbohydrates 8.5 g
+Fiber 1.2 g
+Fat 1.2 g
+Cholesterol 0 mg
+Sodium 156.4 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/baked-buckwheat-puri-healthy-kuttu-ki-puri-42660r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 32449</t>
+  </si>
+  <si>
+    <t>Moong Dal Ki Chaat (100 Calorie Snacks)</t>
+  </si>
+  <si>
+    <t>Zero Oil Snacks</t>
+  </si>
+  <si>
+    <t>For Moong Dal ki Chaat
+1/2 cup yellow moong dal (split yellow gram)
+salt to taste
+1/2 cup grated carrot
+1/2 cup pomegranate (anar)
+1/2 cup chopped spring onions
+1/4 cup chopped raw mangoes
+2 tbsp finely chopped mint leaves (phudina)
+2 tbsp finely chopped coriander (dhania)
+2 tsp finely chopped green chillies
+1 tsp chaat masala
+4 tsp lemon juice</t>
+  </si>
+  <si>
+    <t>Method
+For moong dal ki chaat
+To make moong dal ki chaat, clean, wash and soak the moong dal in enough water for ½ hour and drain well.
+Combine 3 cups of water, moong dal and salt in a deep non-stick pan and cook it on a medium flame till it is half done, while stirring occasionally. Ensure that each grain of the dal is separate.
+Strain the dal using a strainer and keep aside to cool for 10 minutes.
+Combine all the ingredients, including the moong dal, in a large bowl and toss well.
+Serve the moong dal ki chaat immediately.</t>
+  </si>
+  <si>
+    <t>Energy 100 cal
+Protein 5.5 g
+Carbohydrates 18.8 g
+Fiber 3.3 g
+Fat 0.4 g
+Cholesterol 0 mg
+Sodium 10.8 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/moong-dal-ki-chaat-100-calorie-snacks-32449r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6212</t>
+  </si>
+  <si>
+    <t>Ginger Melon Juice, Ginger Watermelon Juice</t>
+  </si>
+  <si>
+    <t>Kidney Stone Diet</t>
+  </si>
+  <si>
+    <t>For Ginger Melon Juice
+2 cups watermelon (tarbuj) cubes
+12 mm piece ginger (adrak) , finely chopped
+1/2 tsp lemon juice
+12 ice-cubes</t>
+  </si>
+  <si>
+    <t>Method
+How to make ginger melon juice in a mixer
+To make ginger melon juice in a mixer, combine the watermelon, ginger, lemon juice and ice-cubes in a mixer jar and blend till smooth.
+Serve immediately.
+How to make in a juicer (hopper)
+To make ginger melon juice in a juicer (hopper), add watermelon cubes and ginger pieces a few at a time in the juicer / hopper.
+Add 6 ice-cubes in each of the 2 glasses and pour equal quantities of juice over it. Note that some amount of fiber will be lost while making juice in a juicer.
+Serve immediately.</t>
+  </si>
+  <si>
+    <t>Energy 53 cal
+Protein 0.7 g
+Carbohydrates 11 g
+Fiber 2 g
+Fat 0.7 g
+Cholesterol 0 mg
+Sodium 86.4 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/ginger-melon-juice-ginger-watermelon-juice-6212r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 38475</t>
+  </si>
+  <si>
+    <t>Oats Idli</t>
+  </si>
+  <si>
+    <t>Hypothyroidism Diet</t>
+  </si>
+  <si>
+    <t>For Oats Idli
+1 cup quick-cooking rolled oats
+1/4 cup urad dal (split black lentils)
+2 tbsp curd (dahi)
+1 tsp ginger-green chilli paste
+salt to taste
+1 tsp fruit salt
+1/2 tsp oil for greasing
+For Serving With Oats Idli
+sambhar</t>
+  </si>
+  <si>
+    <t>Method
+For oats idli
+To make oats idli, combine the oats and urad dal and blend in a mixer to a smooth powder.
+Add 1 cups of water, curd, ginger- green chilli paste and salt and mix well to make a batter of pouring consistency.
+Cover and keep aside to rest for 1 hour.
+Mix the batter well, add the fruit salt and 2 tsp of water and mix it gently.
+Grease the idli moulds using oil and put spoonfuls of batter into them.
+Steam in an idli steamer for 10 to 12 minutes or till they are cooked.
+Demould the oats idlis and serve idli immediately with sambhar.</t>
+  </si>
+  <si>
+    <t>Energy 30 cal
+Protein 1.6 g
+Carbohydrates 5 g
+Fiber 0.9 g
+Fat 0.5 g
+Cholesterol 0 mg
+Sodium 1.3 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/oats-idli-38475r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 40748</t>
+  </si>
+  <si>
+    <t>Zucchini, Bell Pepper and Sprouted Moong Salad</t>
+  </si>
+  <si>
+    <t>1/4 cup finely chopped zucchini (unpeeled)
+1/4 cup finely chopped red capsicum
+1/4 cup finely chopped yellow capsicum
+1/4 cup finely chopped green capsicum
+2 cups parboiled sprouted moong (whole green gram)
+3/4 cup chopped apple (unpeeled and deseeded)
+1 tbsp olive oil
+2 tsp lemon juice
+salt and to taste</t>
+  </si>
+  <si>
+    <t>Method
+Combine all the ingredients in a deep bowl and toss well. Serve immediately.</t>
+  </si>
+  <si>
+    <t>Energy 161 cal
+Protein 8 g
+Carbohydrates 22.6 g
+Fiber 6.6 g
+Fat 4.4 g
+Cholesterol 0 mg
+Sodium 16.5 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/zucchini-bell-pepper-and-sprouted-moong-salad-40748r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 36983</t>
+  </si>
+  <si>
+    <t>Oats Khichdi</t>
+  </si>
+  <si>
+    <t>For Oats Khichdi
+1/2 cup quick cooking rolled oats
+2 tbsp yellow moong dal (split yellow gram) , washed and drained
+1 1/2 tsp oil
+1/2 tsp green chilli paste
+1 tsp garlic (lehsun) paste
+a pinch of turmeric powder (haldi)
+salt to taste
+For Serving With Oats Khichdi
+low-fat curd (dahi)</t>
+  </si>
+  <si>
+    <t>14 mins</t>
+  </si>
+  <si>
+    <t>Method
+For oats khichdi
+To make oats khichdi, heat the oil in a pressure cooker, add the green chilli paste, garlic paste and turmeric powder and sauté on a medium flame for a few seconds.
+Add the oats and yellow moong dal and sauté on a medium flame for 2 to 3 minutes
+Add 2 cups of hot water and salt, mix well and pressure cook for 2 whistles.
+Allow the steam to escape before opening the lid.
+Serve oats khichdi immediately with low-fat curds.
+Handy tip:
+Serving this oats khichdi immediately is important to avoid it being lumpy and sticky.</t>
+  </si>
+  <si>
+    <t>Energy 157 cal
+Protein 6.6 g
+Carbohydrates 20.7 g
+Fiber 3.1 g
+Fat 5.4 g
+Cholesterol 0 mg
+Sodium 3.8 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/oats-khichdi-36983r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22591</t>
+  </si>
+  <si>
+    <t>Zucchini and Carrot Clear Soup</t>
+  </si>
+  <si>
+    <t>Weight Loss Hypothyroidism Diet</t>
+  </si>
+  <si>
+    <t>Zucchini and Carrot Clear Soup
+1/2 cup sliced zucchini
+1/2 cup peeled and sliced carrots
+2 tsp olive oil
+2 tbsp chopped onions
+2 tsp chopped garlic (lehsun)
+1/2 tsp baharat or garam masala
+1/4 cup chopped tomatoes
+2 tsp chopped celery (ajmoda)
+4 cups vegetable stock
+2 tbsp chopped parsley
+salt to taste
+freshly ground black peppercorns (kalimirch) to taste</t>
+  </si>
+  <si>
+    <t>Method
+Zucchini and carrot clear soup
+To make zucchini carrot clear soup, heat the olive oil in a pan add the onions and garlic and sauté for one minute.
+Add the baharat or garam masala, carrots, zucchini, tomatoes and celery and sauté for another 2 minutes.
+Add the vegetable stock, salt and pepper.
+Cook on medium heat for 10 minutes or till the vegetables are cooked. Add parsley and mix well.
+Serve zucchini carrot clear soup hot with pita bread or crusty bread.</t>
+  </si>
+  <si>
+    <t>Energy 65 cal
+Protein 1.6 g
+Carbohydrates 8.9 g
+Fiber 3 g
+Fat 2.7 g
+Cholesterol 0 mg
+Sodium 35.6 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/zucchini-and-carrot-clear-soup-22591r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 42353</t>
+  </si>
+  <si>
+    <t>Masoor Dal Recipe</t>
+  </si>
+  <si>
+    <t>Diabetes Hypothyroidism Diet</t>
+  </si>
+  <si>
+    <t>3/4 cup masoor (split red lentil) dal
+1/4 tsp turmeric powder (haldi)
+1/4 tsp salt
+1 1/2 tsp oil
+1/2 tsp cumin seeds (jeera)
+1 tsp finely chopped ginger (adrak)
+1/4 cup chopped onions
+1/4 tsp garlic (lehsun) paste
+1/4 tsp garam masala
+1/4 tsp chilli powder
+1/4 tsp asafoetida (hing)</t>
+  </si>
+  <si>
+    <t>Method
+Combine the masoor dal, turmeric powder, salt and 1 cup of water in a pressure cooker, mix well and pressure cook for 3 whistles.
+Allow the steam to escape before opening the lid.
+Add 2½ cups of water and whisk it well using a whisk till smooth. Keep aside.
+Heat the oil in a deep non-stick pan add the cumin seeds and ginger and sauté on a medium flame for few seconds.
+Add the onion and sauté on a medium flame for 1 minute.
+Lower the flame add the garlic paste, garam masala, chilli powder, asafoetida and 1 tbsp water and sauté for few seconds.
+Add the whisked dal water mixture, mix well and cook on a medium flame for 2 to 3 minute, while stirring occasionally.
+Switch off the flame, add the lemon juice and mix well.
+Serve hot.</t>
+  </si>
+  <si>
+    <t>Energy 120 cal
+Protein 7.3 g
+Carbohydrates 17.8 g
+Fiber 3 g
+Fat 2.2 g
+Cholesterol 0 mg
+Sodium 196.1 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/masoor-dal-recipe-42353r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 41199</t>
+  </si>
+  <si>
+    <t>Mixed Sprouts and Mint Soup</t>
+  </si>
+  <si>
+    <t>Indian Acidity Soups</t>
+  </si>
+  <si>
+    <t>For Mixed Sprouts and Mint Soup
+2 cups mixed sprouts
+1/4 cup finely chopped mint leaves (phudina)
+1 cup roughly chopped tomatoes
+1/2 cup roughly chopped onions
+1 tbsp roughly chopped garlic (lehsun)
+salt and to taste
+1 tbsp lemon juice</t>
+  </si>
+  <si>
+    <t>Method
+For mixed sprouts and mint soup
+To make mixed sprouts and mint soup, combine the mixed sprouts, tomatoes, onions, garlic and 1½ cups of water in a pressure cooker, mix well and pressure cook for 3 whistles.
+Allow the steam to escape before opening the lid.
+Cool and blend in a mixer till smooth using 2½ cups of water.
+Transfer the mixture into a deep non-stick pan and add the salt and pepper. Mix well and cook on a medium flame for 3 minutes, while stirring occasionally.
+Switch off the flame, add the mint leaves and lemon juice and mix well.
+Serve the mixed sprouts and mint soup hot.</t>
+  </si>
+  <si>
+    <t>Energy 69 cal
+Protein 3.9 g
+Carbohydrates 12.1 g
+Fiber 3.3 g
+Fat 0.5 g
+Cholesterol 0 mg
+Sodium 7 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/mixed-sprouts-and-mint-soup-41199r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 40899</t>
+  </si>
+  <si>
+    <t>Roasted Mushroom and Coloured Capsicum Salad</t>
+  </si>
+  <si>
+    <t>2 cups mushrooms (khumbh)
+1 medium red capsicum
+1 medium green capsicum
+1 medium yellow capsicum
+1 tsp dried rosemary or dried mixed herbs
+1/2 tsp dried thyme
+1 1/2 tsp lemon juice
+salt to taste</t>
+  </si>
+  <si>
+    <t>Method
+Wash, clean and dry the mushrooms and place them on a baking tray and bake in a pre-heated oven at 200°c (400°f) for 11 minutes or till the mushrooms turn light brown in colour, while turning them once after 6 minutes. Keep aside to cool slightly.
+Once they are slightly cooled, cut the stems of the mushrooms and discard them.
+Cut the mushrooms into cubes and keep aside.
+Pierce the red capsicum with a fork and roast it over an open flame till it turns black from all the sides.
+Cool, wash it in cold water and remove the burnt skin, stem and seeds and discard them. Cut the capsicum into cubes and keep aside.
+Repeat steps 4 and 5 for green and yellow capsicum.
+Combine the mushroom and capsicum cubes in a deep bowl, add the rosemary, thyme, lemon juice and salt and toss well.
+Serve immediately.</t>
+  </si>
+  <si>
+    <t>Energy 29 cal
+Protein 1.7 g
+Carbohydrates 5.2 g
+Fiber 2.2 g
+Fat 0.4 g
+Cholesterol 0 mg
+Sodium 3.7 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/roasted-mushroom-and-coloured-capsicum-salad-40899r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 39020</t>
+  </si>
+  <si>
+    <t>Carrot and Red Pepper Juice</t>
+  </si>
+  <si>
+    <t>Healthy Indian Drinks and Juices</t>
+  </si>
+  <si>
+    <t>For Carrot and Red Pepper Juice
+3/4 cup peeled carrot cubes
+3/4 cup red capscium cubes
+1 cup deseeded tomato cubes , see handy tip
+10 to 12 ice-cubes</t>
+  </si>
+  <si>
+    <t>Method
+Carrot and red pepper juice in vitamix
+Combine the carrots cubes, capsicum cubes, tomato cubes, ½ cup of water and ice-cubes in a high quality blender jar (like vitamix) and blend well.
+Serve immediately.
+Carrot and red pepper juice in juicer (hopper)
+Add the carrot cubes, capsicum cubes and tomato cubes a few at a time in a juicer (hopper).
+Add 2 to 3 ice-cubes in each of the 4 glasses and pour equal quantities of juice over it. Note that some amount of fiber will be lost while making juice in a juicer.
+Serve immediately.
+Handy tip:
+2 tomatoes will give approx. 1 cup of deseeded tomato cubes.</t>
+  </si>
+  <si>
+    <t>Energy 17 cal
+Protein 0.7 g
+Carbohydrates 3.3 g
+Fiber 1.5 g
+Fat 0.2 g
+Cholesterol 0 mg
+Sodium 8.4 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/carrot-and-red-pepper-juice-39020r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 40846</t>
+  </si>
+  <si>
+    <t>Red Capsicum Carrot and Apple Juice</t>
+  </si>
+  <si>
+    <t>Indian Cancer Patients</t>
+  </si>
+  <si>
+    <t>For Red Capsicum Carrot and Apple Juice
+1 cup red capscium cubes
+1 cup peeled carrot cubes
+1 cup apple cubes
+10 to 12 ice-cubes</t>
+  </si>
+  <si>
+    <t>Method
+Red capsicum, carrot and apple juice in vitamix
+To make red capsicum, carrot and apple juice, combine the red capsicum cubes, carrot cubes, apple cubes, 1 cup of water and ice cubes in a high quality blender jar (like vitamix) and blend well till smooth and frothy.
+Serve immediately.
+Red capsicum, carrot and apple juice in juicer
+Add the red capsicum cubes, carrot cubes and apple cubes a few at a time in the hopper.
+Add 5 to 6 ice-cubes in each of the 2 glasses and pour equal quantities of juice over it. Note that some amount of fiber will be lost while making juice in a juicer.
+Serve the red capsicum, carrot and apple juice immediately.
+Handy tip:
+This recipe makes use of unpeeled apples, hence take care to clean and wash them well before chopping, to get rid of dirt, germs and chemical residues.</t>
+  </si>
+  <si>
+    <t>Energy 32 cal
+Protein 0.6 g
+Carbohydrates 6.8 g
+Fiber 2.3 g
+Fat 0.3 g
+Cholesterol 0 mg
+Sodium 14.1 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/red-capsicum-carrot-and-apple-juice-40846r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 36892</t>
+  </si>
+  <si>
+    <t>Apple Carrot Juice</t>
+  </si>
+  <si>
+    <t>Fresh Juices</t>
+  </si>
+  <si>
+    <t>For Apple Carrot Juice
+2 cups carrot peeled and cut into thick strips
+1 1/4 cups unpeeled apple wedges
+1/2 tsp roughly chopped ginger (adrak)
+For Serving With Apple Carrot Juice
+10 to 12 ice-cubes</t>
+  </si>
+  <si>
+    <t>Method
+Apple carrot juice in blender
+Combine the carrots cubes, apple cubes, ginger (adrak),1 cup of water and 10 to 12 ice-cubes in a high quality blender jar (like vitamix) and blend well.
+Serve immediately.
+Apple carrot juice in juicer
+Add the carrot cubes, apple cubes and ginger a few at a time in a juicer (hopper).
+Add 2 to 3 ice-cubes in each of the 4 small glasses or 2 big glasses and pour equal quantities of juice over it. Note that some amount of fiber will be lost while making juice in a juicer.
+Serve immediately.</t>
+  </si>
+  <si>
+    <t>Energy 103 cal
+Protein 1.3 g
+Carbohydrates 23.1 g
+Fiber 7.9 g
+Fat 0.6 g
+Cholesterol 0 mg
+Sodium 65.2 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/apple-carrot-juice-36892r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 40441</t>
+  </si>
+  <si>
+    <t>Minty Apple Salad</t>
+  </si>
+  <si>
+    <t>For Minty Apple Salad
+1/4 cup finely chopped mint leaves (phudina)
+3 cups apple cubes
+1 tsp lemon juice
+1 tsp ginger (adrak) juice , refer handy tip
+1 tsp honey
+salt and to taste</t>
+  </si>
+  <si>
+    <t>Method
+For minty apple salad
+Combine all the ingredients in a deep bowl and toss well.
+Serve the minty apple salad immediately.
+Handy tip:
+2 tbsp of grated ginger when placed in a muslin cloth and squeezed gives 2 tsp of ginger juice.</t>
+  </si>
+  <si>
+    <t>Energy 81 cal
+Protein 0.4 g
+Carbohydrates 18.4 g
+Fiber 4 g
+Fat 0.7 g
+Cholesterol 0 mg
+Sodium 32.7 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/minty-apple-salad-40441r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7534</t>
+  </si>
+  <si>
+    <t>Dry Masala Chana Dal, Jain Cucumber Chana Dal Sabzi</t>
+  </si>
+  <si>
+    <t>Non-stick Pan</t>
+  </si>
+  <si>
+    <t>For Dry Masala Chana Dal
+1/2 cup cucumber cubes
+3/4 cup chana dal (split bengal gram)
+1 tsp cumin seeds (jeera)
+1 tsp green chilli paste
+a pinch of turmeric powder (haldi)
+1/2 tsp chilli powder
+1 tbsp oil
+salt to taste</t>
+  </si>
+  <si>
+    <t>Method
+For dry masala chana dal
+To make dry masala chana dal, wash and soak the chana dal in enough hot water in a deep bowl for 1 hour. Drain and keep aside.
+Heat the oil in a deep non-stick pan, add the cumin seeds and sauté on a medium flame for 30 seconds.
+Add the soaked chana dal, green chilli paste, turmeric powder, chilli powder and ¼ cup water, mix well and cover and cook on a medium flame for 6 minutes, while stirring occasionally.
+Add the cucumber, salt and more ¼ cup water, mix well and cover and cook on a medium flame for 3 minutes, while stirring occasionally.
+Serve the dry masala chana dal hot.</t>
+  </si>
+  <si>
+    <t>Energy 234 cal
+Protein 10.5 g
+Carbohydrates 30.4 g
+Fiber 8.2 g
+Fat 7.8 g
+Cholesterol 0 mg
+Sodium 38.7 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/dry-masala-chana-dal-jain-cucumber-chana-dal-sabzi-7534r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 42022</t>
+  </si>
+  <si>
+    <t>Bengali Style Veg Chops, Healthy Low Salt Snack</t>
+  </si>
+  <si>
+    <t>High Blood Pressure Hypothyroidism Diet</t>
+  </si>
+  <si>
+    <t>1/4 cup finely chopped onions
+1/2 cup grated carrot
+1/4 cup grated beetroot
+1/4 cup boiled and mashed potatoes
+1/2 tsp fennel seeds (saunf)
+1/2 tsp cumin seeds (jeera)
+1/2 tsp coriander (dhania) seeds
+1 tsp oil
+1/2 tsp ginger (adrak) paste
+1 tsp finely chopped green chillies
+1/2 tsp chilli powder
+1/4 tsp dried mango powder (amchur)
+1/4 tsp salt
+1/4 tsp freshly ground black pepper (kalimirch)
+1 tsp oil brush (for greasing) and cooking</t>
+  </si>
+  <si>
+    <t>Method
+Combine the fennel seeds, cumin seeds and coriander seeds in a mortal pestle (khalbatta) till coarse. Keep aside.
+Heat the oil in a broad non-stick pan, add the ginger paste and green chillies and sauté on a medium flame for 30 seconds.
+Add the onions and sauté on a medium flame for 1 minute.
+Add the carrot and beetroot and sauté on a medium flame for 1 minute.
+Add the chilli powder, prepared coarsely crushed powder, dried mango powder, salt and 1 tbsp of water, mix well and cook on a medium flame for 30 seconds.
+Transfer the mixture into a big plate, cool slightly, add the potatoes and pepper powder and mix very well.
+Divide the mixture into 12 equal portions and roll each portion into an oblong shape.
+Heat a non-stick tava (griddle) and grease it using the remaining ½ tsp of oil.
+Place the chops on it and cook using ½ tsp of oil till they turn golden brown in colour from both the sides.
+Serve immediately.</t>
+  </si>
+  <si>
+    <t>Energy 13 cal
+Protein 0.1 g
+Carbohydrates 1.2 g
+Fiber 0.3 g
+Fat 0.8 g
+Cholesterol 0 mg
+Sodium 67 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/bengali-style-veg-chops-healthy-low-salt-snack-42022r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 40706</t>
+  </si>
+  <si>
+    <t>Sprouted Matki Uttapam</t>
+  </si>
+  <si>
+    <t>Pregnancy Third Trimester Foods</t>
+  </si>
+  <si>
+    <t>For Sprouted Matki Uttapam
+1 1/2 cups sprouted matki (moath beans)
+1/4 cup besan (bengal gram flour)
+1/4 cup finely chopped coriander (dhania)
+1/4 cup chopped tomatoes
+1/4 cup grated carrot
+2 tsp ginger-green chilli paste
+1/4 tsp cumin seeds (jeera)
+1/4 tsp asafoetida (hing)
+salt to taste
+2 tsp oil for greasing and cooking</t>
+  </si>
+  <si>
+    <t>Method
+For sprouted matki uttapam
+To make sprouted matki uttapam, combine the sprouted matki and ½ cup of water in a mixer and blend till smooth.
+Transfer the mixture into a deep bowl, add besan, coriander, tomatoes, carrot, ginger-green chilli paste, cumin seeds, hing, salt and mix well.
+Grease a non-stick pan with ¼ tsp of oil.
+Pour a ladleful of the batter and spread in a circular motion to make a 125 mm. (5") diameter thick circle.
+Cook till they turn brown in colour from both the sides using a little oil.
+Serve the sprouted matki uttapam immediately with coconut chutney.</t>
+  </si>
+  <si>
+    <t>Energy 92 cal
+Protein 5.2 g
+Carbohydrates 13.2 g
+Fiber 1.7 g
+Fat 2.1 g
+Cholesterol 0 mg
+Sodium 11 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/sprouted-matki-uttapam-40706r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 41758</t>
+  </si>
+  <si>
+    <t>Oats Appe, Oats Vegetable Appe</t>
+  </si>
+  <si>
+    <t>Appe Mould</t>
+  </si>
+  <si>
+    <t>For Oats Appe
+1/2 cup powered quick cooking rolled oats
+1/2 cup finely chopped spring onions whites and greens
+1/2 cup urad dal (split black lentils)
+2 tsp crushed black pepper (kalimirch)
+salt to taste
+2 tsp oil for greasing and cooking</t>
+  </si>
+  <si>
+    <t>Method
+For oats appe
+To make oats appe, soak the urad dal in enough water in a deep bowl and keep aside to soak for 1 hour. Drain well.
+Blend the urad dal in a mixer using ¼ cup of water till smooth.
+Transfer the mixture into a deep bowl, add the oats, spring onions, crushed black pepper and salt and mix very well.
+Heat an appe mould on a medium flame and grease it using ¼ tsp of oil. Pour 1 tbsp of the batter into each mould and cook using ¼ tsp of oil till the lower surface becomes golden brown and then turn each appe upside down using a fork so as to cook them from the other side as well.
+Repeat step 4 to make more appes.
+Serve the oats appe immediately.</t>
+  </si>
+  <si>
+    <t>Energy 43 cal
+Protein 2.3 g
+Carbohydrates 6.3 g
+Fiber 1.2 g
+Fat 1 g
+Cholesterol 0 mg
+Sodium 3.1 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/oats-appe-oats-vegetable-appe-41758r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 41653</t>
+  </si>
+  <si>
+    <t>Oats Nimki, Low Salt Recipe</t>
+  </si>
+  <si>
+    <t>1/2 cup powdered oats
+1/2 cup whole wheat flour (gehun ka atta)
+1/4 tsp roasted and crushed cumin seeds (jeera)
+1/4 crushed peppercorns (kalimirch)
+1/8 tsp salt
+2 tsp oil
+whole wheat flour (gehun ka atta) for rolling</t>
+  </si>
+  <si>
+    <t>Method
+Combine all the ingredients in a deep bowl and knead into semi-stiff dough using enough water.
+Divide the dough into 6 equal portions.
+Roll out each portion into a thin round circle of 150 mm. (6”) diameter using a little whole wheat flour for rolling.
+Cut each circle into 8 equal size long strips and keep aside. You will get 48 strips in all.
+Heat a non-stick tava (griddle) and cook the strips, a few at a time, on hot tava (griddle), while pressing them using folded muslin cloth or khakhra press, till they turn crisp and golden brown in colour from both the sides.
+Cool completely and serve or store in an air-tight container</t>
+  </si>
+  <si>
+    <t>Energy 76 cal
+Protein 2.4 g
+Carbohydrates 11.6 g
+Fiber 0.9 g
+Fat 2.3 g
+Cholesterol 0 mg
+Sodium 66.8 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/oats-nimki-low-salt-recipe-41653r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 40377</t>
+  </si>
+  <si>
+    <t>Baked Masala Sev</t>
+  </si>
+  <si>
+    <t>Oven</t>
+  </si>
+  <si>
+    <t>For Baked Masala Sev
+1 cup besan (bengal gram flour)
+1/4 cup fresh tomato pulp
+1/4 tsp asafoetida (hing)
+1/4 tsp turmeric powder (haldi)
+1 1/2 tsp chilli powder
+1/4 tsp freshly ground black pepper (kalimirch)
+1 tsp oil
+salt to taste</t>
+  </si>
+  <si>
+    <t>Method
+For baked masala sev
+To make baked masala sev combine gram flour, tomato pulp, hing, haldi, chilli powder, salt, pepper and oil in a deep bowl, mix well and knead into a soft dough without using any water.
+Shape the dough into a cylindrical roll, fill the dough into the “sev press” and press out strands onto a greased baking tray.
+Bake in a preheated oven at 200°c (400°f) for 14 minutes, turn them over after 9 minutes then break into pieces and bake again for 5 minutes, while tossing twice in between.
+Cool, break them into pieces.
+Store baked masala sev in an air-tight container and use as required.</t>
+  </si>
+  <si>
+    <t>Energy 24 cal
+Protein 1.2 g
+Carbohydrates 3.4 g
+Fiber 0.9 g
+Fat 0.6 g
+Cholesterol 0 mg
+Sodium 4.5 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/baked-masala-sev-40377r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 41505</t>
+  </si>
+  <si>
+    <t>Minty Quinoa, Ibs Recipe</t>
+  </si>
+  <si>
+    <t>Iron Deficiency (Anaemia) Hypothyroidism Diet</t>
+  </si>
+  <si>
+    <t>For Minty Quinoa
+1/4 cup finely chopped mint leaves (phudina) leaves
+1 cup quinoa , washed and drained
+2 tsp olive oil
+1/2 cup chopped carrot
+1/4 cup chopped celery (ajmoda)
+1/2 tsp finely chopped green chillies
+1/4 cup chopped red pumpkin (bhopla / kaddu)
+2 bay leaves (tejpatta)
+salt to taste
+freshly ground black pepper (kalimirch) to taste</t>
+  </si>
+  <si>
+    <t>Method
+For minty quinoa for ibs
+To make minty quinoa heat oil in a deep non-stick pan, add the carrots, celery and green chillies sauté on a medium flame for 2 minutes.
+Add the quinoa, red pumpkin, bayleaves, salt, pepper powder and 2½ cups of water and mix well. Cover with a lid and cook on a slow flame for 15 to 16 minutes, while stirring occasionally.
+Add the mint leaves and mix well.
+Serve minty quinoa immediately.</t>
+  </si>
+  <si>
+    <t>Energy 208 cal
+Protein 7 g
+Carbohydrates 36.7 g
+Fiber 11 g
+Fat 5.5 g
+Cholesterol 0 mg
+Sodium 14.6 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/minty-quinoa-ibs-recipe-41505r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 41364</t>
+  </si>
+  <si>
+    <t>Avocado and Tomato Salad, Healthy and Quick Salad</t>
+  </si>
+  <si>
+    <t>B Vitamins</t>
+  </si>
+  <si>
+    <t>1 1/2 cups sliced avocados
+1 cup deseeded and sliced tomatoes
+To Be Mixed Into A Dressing
+1 tbsp olive oil
+1/2 tsp mustard (rai / sarson) powder
+1 tsp lemon juice
+salt and to taste</t>
+  </si>
+  <si>
+    <t>Method
+Combine all the ingredients along with the dressing in a deep bowl and toss well.
+Serve immediately.</t>
+  </si>
+  <si>
+    <t>Energy 269 cal
+Protein 2.1 g
+Carbohydrates 3.3 g
+Fiber 1.1 g
+Fat 27.5 g
+Cholesterol 0 mg
+Sodium 7.6 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/avocado-and-tomato-salad-healthy-and-quick-salad-41364r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 36414</t>
+  </si>
+  <si>
+    <t>Bean Sprouts and Suva Tossed Salad</t>
+  </si>
+  <si>
+    <t>Vegan</t>
+  </si>
+  <si>
+    <t>For Bean Sprouts and Suva Tossed Salad
+2 cups bean sprouts
+1/4 cup finely chopped dill leaves
+1/2 cup chopped tomatoes
+1 tbsp lemon juice
+1/4 cup chopped basil
+salt to taste</t>
+  </si>
+  <si>
+    <t>Method
+For bean sprouts and suva tossed salad
+To make bean sprouts and suva tossed salad, combine all the ingredients in a deep bowl and toss well.
+Serve immediately.</t>
+  </si>
+  <si>
+    <t>Energy 21 cal
+Protein 1.5 g
+Carbohydrates 4 g
+Fiber 1.3 g
+Fat 0.2 g
+Cholesterol 0 mg
+Sodium 5.9 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/bean-sprouts-and-suva-tossed-salad-36414r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 39013</t>
+  </si>
+  <si>
+    <t>Muskmelon and Pineapple Juice</t>
+  </si>
+  <si>
+    <t>2 cups chilled and roughly chopped muskmelon (kharbooja)
+4 cups chilled and roughly chopped pineapple
+For Serving
+8 ice-cubes</t>
+  </si>
+  <si>
+    <t>Method
+Add the muskmelon and pineapple a few at a time in a hopper.
+Pour equal quantities of the juice into 4 individual glasses.
+Serve immediately topped with 2 ice-cubes in each glass.</t>
+  </si>
+  <si>
+    <t>Energy 80 cal
+Protein 0.8 g
+Carbohydrates 18.5 g
+Fiber 4.7 g
+Fat 0.3 g
+Cholesterol 0 mg
+Sodium 130 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/muskmelon-and-pineapple-juice-39013r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6213</t>
+  </si>
+  <si>
+    <t>Apple Magic, Lemony Apple Juice</t>
+  </si>
+  <si>
+    <t>Pregnancy</t>
+  </si>
+  <si>
+    <t>Juicer Method
+3 cups apple cubes
+2 tsp lemon juice
+crushed ice for serving , optional</t>
+  </si>
+  <si>
+    <t>Method
+Juicer method
+Add the apple cubes a few at a time in the juicer.
+Add the lemon juice and mix well.
+Add some crushed ice in 2 individual glasses and pour equal quantities of the juice over it.
+Serve the lemony apple juice immediately.
+Mixer method
+This recipe doesn’t turn out good in a mixer because the texture of ingredients like apple is very hard.
+Handy tip:
+This recipe makes use of unpeeled fruits and vegetables, hence take care to clean and wash them well before chopping, to get rid of dirt, germs and chemical residues.</t>
+  </si>
+  <si>
+    <t>Energy 108 cal
+Protein 0.4 g
+Carbohydrates 24.4 g
+Fiber 5.7 g
+Fat 1 g
+Cholesterol 0 mg
+Sodium 48.9 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/apple-magic-lemony-apple-juice-6213r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22206</t>
+  </si>
+  <si>
+    <t>Bhindi Masala</t>
+  </si>
+  <si>
+    <t>High Cholestrol Hypothyroidism Diet</t>
+  </si>
+  <si>
+    <t>For Bhindi Masala
+20 tender ladies finger (bhindi)
+2 tbsp besan (bengal gram flour)
+2 tsp oil
+For The Bhindi Masala Paste
+1/2 cup roughly chopped onions
+1 cup chopped coriander (dhania)
+2 tsp ginger-green chilli paste
+1/2 tsp turmeric powder (haldi)
+1 tbsp coriander-cumin seeds (dhania-jeera) powder
+1 tsp garam masala
+2 tsp roasted sesame seeds (til)
+1 tbsp lemon juice
+salt to taste
+For Serving With Bhindi Masala
+rotis/parathas</t>
+  </si>
+  <si>
+    <t>Method
+For the bhindi masala paste
+Combine all the ingredients and 2 tbsp of water in a mixer and blend till smooth.
+Transfer the mixture into a deep bowl, add the besan and mix well. Keep aside.
+How to proceed to make bhindi masala
+To make bhindi masala, wash, dry and slit the bhindi lengthwise.
+Stuff each bhindi with a little prepared paste. Keep the remaining paste aside.
+Heat a non-stick tava (griddle), put the remaining paste and 2 tbsp of water and sauté on a medium flame for 2 minutes.
+Add the stuffed bhindis and sauté on a medium flame for 4 minutes.
+Cover with a lid and cook on a medium flame for 6 to 8 minutes, while stirring occasionally.
+Serve the bhindi masala hot with rotis or parathas.</t>
+  </si>
+  <si>
+    <t>Energy 83 cal
+Protein 3.6 g
+Carbohydrates 14.2 g
+Fiber 3.6 g
+Fat 1.4 g
+Cholesterol 0 mg
+Sodium 15.7 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/bhindi-masala-22206r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8651</t>
+  </si>
+  <si>
+    <t>Avocado Dip, Avocado Jain Dip</t>
+  </si>
+  <si>
+    <t>Gout Indian Recipes</t>
+  </si>
+  <si>
+    <t>1 cup mashed ripe avocado
+1 tsp lemon juice
+2 tbsp chopped tomatoes
+1/2 tsp chopped green chillies
+salt to taste
+For Serving
+corn chips</t>
+  </si>
+  <si>
+    <t>Method
+Combine all the ingredients in a deep bowl and mix well.
+Serve with corn chips.</t>
+  </si>
+  <si>
+    <t>Energy 31 cal
+Protein 0.3 g
+Carbohydrates 0.3 g
+Fiber 0 g
+Fat 3.3 g
+Cholesterol 0 mg
+Sodium 0.2 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/avocado-dip-avocado-jain-dip-8651r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 38954</t>
+  </si>
+  <si>
+    <t>Fluffy Egg White Masala Omelette</t>
+  </si>
+  <si>
+    <t>Low Carb Indian Snacks</t>
+  </si>
+  <si>
+    <t>3 eggs whites
+1 tsp olive oil
+salt and freshly ground to taste
+For The Masala Vegetables
+1/4 cup finely chopped onions
+1/2 cup red and yellow capsicum chopped
+1/4 cup finely chopped mushrooms (khumbh)
+1/4 cup finely chopped tomatoes
+1/2 tsp finely chopped green chillies
+1 tsp olive oil</t>
+  </si>
+  <si>
+    <t>Method
+For the masala vegetables
+In a pan, heat the olive oil and sauté the onions, capsicums , mushrooms, and green chilli for 1 minute. Add the tomatoes and cook again. Keep aside.
+How to proceed
+Beat the egg whites in a electric beater on a slow for 2 to 3 minutes or until the mixture is thick and frothy.
+Heat the olive oil in a 10 inch pan. Add the beaten egg and cook for a few minutes checking with a spatula to see when the bottom of the egg is done. Then add the cooked masala vegetables in the centre of the omelette. Fold the omelette into half and serve hot with a whole wheat toast.
+Sprinkle fresh pepper on top.</t>
+  </si>
+  <si>
+    <t>Energy 394 cal
+Protein 22 g
+Carbohydrates 8.9 g
+Fiber 2.6 g
+Fat 30.3 g
+Cholesterol 0 mg
+Sodium 9.4 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/fluffy-egg-white-masala-omelette-38954r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 41020</t>
+  </si>
+  <si>
+    <t>Gavar Aur Masoor ki Dal</t>
+  </si>
+  <si>
+    <t>Cancer Dals</t>
+  </si>
+  <si>
+    <t>3/4 cup chopped cluster beans (gavarfali)
+3/4 cup masoor dal (split red lentil) , washed and drained
+2 tsp oil
+1 tsp cumin seeds (jeera)
+1/4 tsp asafoetida (hing)
+1/4 cup finely chopped onions
+1 tsp garlic (lehsun) paste
+1/4 cup finely chopped tomatoes
+3/4 tsp chilli powder
+1/4 tsp turmeric powder (haldi)
+salt to taste</t>
+  </si>
+  <si>
+    <t>28 mins</t>
+  </si>
+  <si>
+    <t>Method
+Combine the masoor dal and 1½ cups of water in a pressure cooker and pressure cook for 3 whistles.
+Allow the steam to escape before opening the lid.
+Add 1½ cups of water and mix well using a whisk. Keep aside.
+Heat the oil in a deep non-stick pan and add the cumin seeds and asafoetida and sauté on a medium flame for a few seconds.
+Add the onions and garlic paste and sauté on a medium flame for 1 minute.
+Add the tomatoes, mix well and cook on a medium flame for 1 minute.
+Add the cluster beans, chilli powder, turmeric powder, salt and ½ cup of water and mix well. Cover with a lid and cook on a medium flame for 6 minutes, while stirring occasionally.
+Add the cooked masoor dal, mix well and cook on a medium flame for another 3 minutes, while stirring occasionally.
+Serve hot.</t>
+  </si>
+  <si>
+    <t>Energy 129 cal
+Protein 7.9 g
+Carbohydrates 20.1 g
+Fiber 4.2 g
+Fat 2.8 g
+Cholesterol 0 mg
+Sodium 3.6 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/gavar-aur-masoor-ki-dal-41020r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1706</t>
+  </si>
+  <si>
+    <t>Dal and Vegetable Idli</t>
+  </si>
+  <si>
+    <t>Hair Growth Hypothyroidism Diet</t>
+  </si>
+  <si>
+    <t>For Dal and Vegetable Idli
+1/2 cup toovar (arhar) dal
+1/4 cup yellow moong dal (split yellow gram)
+1/2 cup chana dal (split bengal gram)
+1 cup chopped fenugreek leaves (methi)
+2 cups chopped coriander (dhania)
+1/4 cup boiled green peas
+1/4 cup grated coconut
+2 tsp chopped green chillies
+1/4 cup chopped onions
+1/4 cup grated carrot
+salt to taste
+oil for greasing</t>
+  </si>
+  <si>
+    <t>Method
+For dal and vegetable idli
+To make dal and vegetable idli, wash and soak the dals together at least 3 hours.
+Drain, add water and grind to a smooth paste.
+Add the fenugreek, coriander, green peas, coconut, green chillies, onion, carrot and salt and mix well.
+Gradually add water as required to make a thick batter. We added a total of 3/4th cup water.
+Just before steaming, add fruit salt and 1 tbsp of water to the batter and mix gently.
+Pour into greased idli moulds and steam for 10 to 12 minutes till done.
+Serve the dal and vegetable idli hot with sambhar and coconut chutney.</t>
+  </si>
+  <si>
+    <t>Energy 49 cal
+Protein 2.8 g
+Carbohydrates 7.5 g
+Fiber 2 g
+Fat 0.9 g
+Cholesterol 0 mg
+Sodium 9.2 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/dal-and-vegetable-idli-1706r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 40134</t>
+  </si>
+  <si>
+    <t>Whole Masoor Salad</t>
+  </si>
+  <si>
+    <t>Protein Rich foods for Pregnancy</t>
+  </si>
+  <si>
+    <t>1/2 cup whole masoor (whole red lentil)
+salt to taste
+1/2 cup deseeded and chopped cucumber
+1/2 cup chopped carrot
+1/4 cup deseeded and chopped tomatoes
+1/2 cup chopped spring onions (whites and greens)
+To Be Mixed Into A Dressing
+1/2 tbsp olive oil
+1 tsp lemon juice
+1/2 tsp finely chopped green chillies
+1/4 tsp freshly ground black pepper (kalimirch)
+salt to taste</t>
+  </si>
+  <si>
+    <t>Method
+Clean, wash and soak the whole masoor in a deep bowl in enough water overnight. Drain well.
+Combine the whole soaked masoor, salt and ½ cup of water in a deep non-stick pan and mix well. Cover with a lid and cook on a medium flame for 8 minutes or till all the water has been evaporated, while stirring occasionally. Keep aside to cool completely.
+Once cooled, transfer the cooked whole masoor into a deep bowl, add all the remaining ingredients and mix well.
+Finally, pour the prepared dressing over it and toss gently.
+Serve immediately.</t>
+  </si>
+  <si>
+    <t>Energy 204 cal
+Protein 11 g
+Carbohydrates 30 g
+Fiber 7.1 g
+Fat 4.5 g
+Cholesterol 0 mg
+Sodium 19.9 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/whole-masoor-salad-40134r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5574</t>
+  </si>
+  <si>
+    <t>Rajma and Urad Dal</t>
+  </si>
+  <si>
+    <t>Frozen Foods Indian Curry</t>
+  </si>
+  <si>
+    <t>For Rajma and Urad Dal
+1/4 cup rajma (kidney beans)
+1/4 cup chana dal (split bengal gram)
+1/2 cup chilkewali urad dal (spit black gram with skin)
+salt to taste
+2 tsp oil
+1 tbsp finely chopped garlic (lehsun)
+1/2 cup finely chopped onions
+1 tsp green chilli paste
+1 cup finely chopped tomatoes
+1 tsp chilli powder
+2 tsp cumin seeds (jeera) powder
+1/4 cup chopped coriander (dhania)
+1 tbsp lemon juice</t>
+  </si>
+  <si>
+    <t>Method
+Clean, wash and soak the rajma, chana and urad dal in a deep bowl with enough water overnight.
+Drain the soaked dals, add 4 cups water and salt, mix well and pressure cook for 4 whistles.
+Allow the steam to escape before opening the lid. Keep aside.
+Heat the oil in a deep non-stick pan, add the garlic, onions and green chilli paste and sauté on a medium flame for 1 minute.
+Add the tomatoes, chilli powder, cumin seeds powder, little salt and 2 tbsp of water, mix well and cook on a medium flame for 2 to 3 minutes, while stirring occasionally.
+Add the cooked dals and coriander, mix well and cook on a medium flame for 2 to 3 minutes, while stirring occasionally.
+Add the lemon juice, mix well and serve hot.</t>
+  </si>
+  <si>
+    <t>Energy 126 cal
+Protein 6.7 g
+Carbohydrates 19.1 g
+Fiber 3.7 g
+Fat 2.5 g
+Cholesterol 0 mg
+Sodium 15.7 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/rajma-and-urad-dal-5574r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4642</t>
+  </si>
+  <si>
+    <t>Muskmelon, Pear and Apple Salad</t>
+  </si>
+  <si>
+    <t>1 1/2 cups chilled muskmelon (kharbooja) cubes
+3/4 cup chilled pear cubes
+3/4 cup chilled apple cubes
+To Be Mixed Into A Parsley Dressing
+1/4 cup finely chopped parsley
+1/2 cup thick low-fat curds (dahi)
+1/4 tsp mustard (rai / sarson) powder
+salt to taste</t>
+  </si>
+  <si>
+    <t>Method
+Combine the muskmelon, pear and apples in a deep bowl and mix well.
+Just before serving, add the parsley dressing and toss well.
+Serve immediately.</t>
+  </si>
+  <si>
+    <t>Energy 45 cal
+Protein 1.3 g
+Carbohydrates 9.3 g
+Fiber 2.3 g
+Fat 0.3 g
+Cholesterol 0 mg
+Sodium 79.6 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/muskmelon-pear-and-apple-salad-4642r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 39642</t>
+  </si>
+  <si>
+    <t>Citrus Watermelon Salad</t>
+  </si>
+  <si>
+    <t>Healthy Fruit Snacks</t>
+  </si>
+  <si>
+    <t>For Citrus Watermelon Salad
+2 cups watermelon (tarbuj) cubes
+1/2 cup orange segments
+1/2 cup sweet lime (mosambi) segments
+1/2 cup pomegranate (anar)
+To Be Mixed Into A Dressing
+2 tsp extra virgin olive oil
+2 tbsp finely chopped parsley
+1 tsp lemon juice
+1/2 tsp sea salt (khada namak)</t>
+  </si>
+  <si>
+    <t>Method
+For citrus watermelon salad
+To make citrus watermelon salad, prepare the parsley lemon extra virgin olive oil dressing by mixing all ingredients.
+In a deep bowl put watermelon (tarbuj) cubes, orange segments, sweet lime (mosambi) segments and pomegranate (anar).
+Add the dressing just before serving. Toss well.
+Serve citrus watermelon salad immediately.</t>
+  </si>
+  <si>
+    <t>Energy 93 cal
+Protein 1.2 g
+Carbohydrates 13.6 g
+Fiber 2.7 g
+Fat 3.8 g
+Cholesterol 0 mg
+Sodium 32.2 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/citrus-watermelon-salad-39642r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 379</t>
+  </si>
+  <si>
+    <t>Chawli, Rajma and Chick Pea Healthy Salad</t>
+  </si>
+  <si>
+    <t>For Chawli , Rajma and Chick Pea Salad
+2 1/4 cups mixed boiled beans (rajma , chawli and chick peas)
+1/2 cup sliced spring onions
+1/2 cup tomato cubes
+1 tsp finely chopped green chillies
+1 tbsp finely chopped coriander (dhania)
+To Be Mixed Into A Dressing
+2 tbsp lemon juice
+2 tsp chaat masala
+1/4 tsp black salt (sanchal)
+salt and to taste
+For The Garnish
+1 tbsp finely chopped coriander (dhania)</t>
+  </si>
+  <si>
+    <t>Method
+For chawli, rajma and chick pea salad
+To make chawli, rajma and chick pea salad, combine all the ingredients (except the dressing) in a deep bowl and mix well.
+Refrigerate for 1 hour or longer.
+Just before serving add the peppy lemon dressing. Toss well.
+Serve healthy three bean chaat salad chilled garnished with coriander.</t>
+  </si>
+  <si>
+    <t>Energy 296 cal
+Protein 20.7 g
+Carbohydrates 50.7 g
+Fiber 14.9 g
+Fat 1.3 g
+Cholesterol 0 mg
+Sodium 165.1 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/chawli-rajma-and-chick-pea-healthy-salad-379r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6210</t>
+  </si>
+  <si>
+    <t>Papaya Coconut Drink</t>
+  </si>
+  <si>
+    <t>For Papaya Coconut Drink
+1 cup papaya cubes
+1/4 cup coconut meat (nariyal ki malai)
+3/4 cup chilled coconut water (nariyal ka pani)
+10 to 12 ice-cubes</t>
+  </si>
+  <si>
+    <t>Method
+For papaya coconut drink
+To make papaya coconut drink, combine the papaya cubes, coconut meat, coconut water and ice cubes in a mixer jar and blend well till smooth.
+Serve the papaya coconut drinkimmediately.
+Handy tip:
+This recipe doesn’t turn out good in a juicer (hopper) because the texture of papaya is very soft.</t>
+  </si>
+  <si>
+    <t>Energy 61 cal
+Protein 1.3 g
+Carbohydrates 11 g
+Fiber 9 g
+Fat 1.4 g
+Cholesterol 0 mg
+Sodium 4.2 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/papaya-coconut-drink-6210r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3600</t>
+  </si>
+  <si>
+    <t>Minty Bean Salad</t>
+  </si>
+  <si>
+    <t>High Blood Pressure</t>
+  </si>
+  <si>
+    <t>2 tbsp finely chopped mint leaves (phudina)
+1 1/2 cups soaked and cooked chawli , refer handy tip
+1/2 cup chopped cucumber
+1/2 cup finely chopped onions
+1/2 cup finely chopped tomatoes
+2 tbsp finely chopped coriander (dhania)
+1/2 tsp finely chopped green chillies
+1/4 tsp black salt (sanchal)
+1/2 tbsp lemon juice
+salt to taste</t>
+  </si>
+  <si>
+    <t>Method
+Combine all the ingredients in a bowl and toss well.
+Serve immediately or refrigerate for 1 hour and serve chilled.
+Handy tip:
+½ cup of raw chawli, when soaked and boiled yields 1½ cups cooked chawli. Ensure not to overcook the chawli for this recipe.</t>
+  </si>
+  <si>
+    <t>Energy 115 cal
+Protein 7.8 g
+Carbohydrates 19.8 g
+Fiber 5.9 g
+Fat 0.4 g
+Cholesterol 0 mg
+Sodium 12.6 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/minty-bean-salad-3600r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5559</t>
+  </si>
+  <si>
+    <t>Rajma Cucumber and Carrot Salad</t>
+  </si>
+  <si>
+    <t>1 cup thinly sliced carrot
+1 cup thinly sliced cucumber
+1/2 cup soaked and boiled rajma (kidney beans)
+1/2 cup sliced spring onions (white and greens)
+To Be Mixed Together Into A Mint Dressing
+2 tbsp finely chopped mint leaves (phudina)
+4 tsp honey
+1 tbsp lemon juice
+salt to taste</t>
+  </si>
+  <si>
+    <t>Method
+Combine all the ingredients for the salad in a bowl, toss well and refrigerate for at least 1 hour.
+Just before serving, add the mint dressing and toss well.
+Serve immediately.</t>
+  </si>
+  <si>
+    <t>Energy 68 cal
+Protein 2.1 g
+Carbohydrates 14.9 g
+Fiber 2.9 g
+Fat 0.3 g
+Cholesterol 0 mg
+Sodium 15 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/rajma-cucumber-and-carrot-salad-5559r</t>
+  </si>
+  <si>
+    <t>No of Recipes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3181,19 +5477,389 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DW11"/>
+  <dimension ref="A1:IK11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+    <sheetView tabSelected="1" topLeftCell="II1" workbookViewId="0">
+      <selection sqref="A1:IK1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" customWidth="true" width="39.0"/>
+    <col min="1" max="3" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:245" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>826</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>2</v>
+      </c>
+      <c r="G1">
+        <v>3</v>
+      </c>
+      <c r="I1">
+        <v>4</v>
+      </c>
+      <c r="K1">
+        <v>5</v>
+      </c>
+      <c r="M1">
+        <v>6</v>
+      </c>
+      <c r="O1">
+        <v>7</v>
+      </c>
+      <c r="Q1">
+        <v>8</v>
+      </c>
+      <c r="S1">
+        <v>9</v>
+      </c>
+      <c r="U1">
+        <v>10</v>
+      </c>
+      <c r="W1">
+        <v>11</v>
+      </c>
+      <c r="Y1">
+        <v>12</v>
+      </c>
+      <c r="AA1">
+        <v>13</v>
+      </c>
+      <c r="AC1">
+        <v>14</v>
+      </c>
+      <c r="AE1">
+        <v>15</v>
+      </c>
+      <c r="AG1">
+        <v>16</v>
+      </c>
+      <c r="AI1">
+        <v>17</v>
+      </c>
+      <c r="AK1">
+        <v>18</v>
+      </c>
+      <c r="AM1">
+        <v>19</v>
+      </c>
+      <c r="AO1">
+        <v>20</v>
+      </c>
+      <c r="AQ1">
+        <v>21</v>
+      </c>
+      <c r="AS1">
+        <v>22</v>
+      </c>
+      <c r="AU1">
+        <v>23</v>
+      </c>
+      <c r="AW1">
+        <v>24</v>
+      </c>
+      <c r="AY1">
+        <v>25</v>
+      </c>
+      <c r="BA1">
+        <v>26</v>
+      </c>
+      <c r="BC1">
+        <v>27</v>
+      </c>
+      <c r="BE1">
+        <v>28</v>
+      </c>
+      <c r="BG1">
+        <v>29</v>
+      </c>
+      <c r="BI1">
+        <v>30</v>
+      </c>
+      <c r="BK1">
+        <v>31</v>
+      </c>
+      <c r="BM1">
+        <v>32</v>
+      </c>
+      <c r="BO1">
+        <v>33</v>
+      </c>
+      <c r="BQ1">
+        <v>34</v>
+      </c>
+      <c r="BS1">
+        <v>35</v>
+      </c>
+      <c r="BU1">
+        <v>36</v>
+      </c>
+      <c r="BW1">
+        <v>37</v>
+      </c>
+      <c r="BY1">
+        <v>38</v>
+      </c>
+      <c r="CA1">
+        <v>39</v>
+      </c>
+      <c r="CC1">
+        <v>40</v>
+      </c>
+      <c r="CE1">
+        <v>41</v>
+      </c>
+      <c r="CG1">
+        <v>42</v>
+      </c>
+      <c r="CI1">
+        <v>43</v>
+      </c>
+      <c r="CK1">
+        <v>44</v>
+      </c>
+      <c r="CM1">
+        <v>45</v>
+      </c>
+      <c r="CO1">
+        <v>46</v>
+      </c>
+      <c r="CQ1">
+        <v>47</v>
+      </c>
+      <c r="CS1">
+        <v>48</v>
+      </c>
+      <c r="CU1">
+        <v>49</v>
+      </c>
+      <c r="CW1">
+        <v>50</v>
+      </c>
+      <c r="CY1">
+        <v>51</v>
+      </c>
+      <c r="DA1">
+        <v>52</v>
+      </c>
+      <c r="DC1">
+        <v>53</v>
+      </c>
+      <c r="DE1">
+        <v>54</v>
+      </c>
+      <c r="DG1">
+        <v>55</v>
+      </c>
+      <c r="DI1">
+        <v>56</v>
+      </c>
+      <c r="DK1">
+        <v>57</v>
+      </c>
+      <c r="DM1">
+        <v>58</v>
+      </c>
+      <c r="DO1">
+        <v>59</v>
+      </c>
+      <c r="DQ1">
+        <v>60</v>
+      </c>
+      <c r="DS1">
+        <v>61</v>
+      </c>
+      <c r="DU1">
+        <v>62</v>
+      </c>
+      <c r="DW1">
+        <v>63</v>
+      </c>
+      <c r="DY1">
+        <v>64</v>
+      </c>
+      <c r="EA1">
+        <v>65</v>
+      </c>
+      <c r="EC1">
+        <v>66</v>
+      </c>
+      <c r="EE1">
+        <v>67</v>
+      </c>
+      <c r="EG1">
+        <v>68</v>
+      </c>
+      <c r="EI1">
+        <v>69</v>
+      </c>
+      <c r="EK1">
+        <v>70</v>
+      </c>
+      <c r="EM1">
+        <v>71</v>
+      </c>
+      <c r="EO1">
+        <v>72</v>
+      </c>
+      <c r="EQ1">
+        <v>73</v>
+      </c>
+      <c r="ES1">
+        <v>74</v>
+      </c>
+      <c r="EU1">
+        <v>75</v>
+      </c>
+      <c r="EW1">
+        <v>76</v>
+      </c>
+      <c r="EY1">
+        <v>77</v>
+      </c>
+      <c r="FA1">
+        <v>78</v>
+      </c>
+      <c r="FC1">
+        <v>79</v>
+      </c>
+      <c r="FE1">
+        <v>80</v>
+      </c>
+      <c r="FG1">
+        <v>81</v>
+      </c>
+      <c r="FI1">
+        <v>82</v>
+      </c>
+      <c r="FK1">
+        <v>83</v>
+      </c>
+      <c r="FM1">
+        <v>84</v>
+      </c>
+      <c r="FO1">
+        <v>85</v>
+      </c>
+      <c r="FQ1">
+        <v>86</v>
+      </c>
+      <c r="FS1">
+        <v>87</v>
+      </c>
+      <c r="FU1">
+        <v>88</v>
+      </c>
+      <c r="FW1">
+        <v>89</v>
+      </c>
+      <c r="FY1">
+        <v>90</v>
+      </c>
+      <c r="GA1">
+        <v>91</v>
+      </c>
+      <c r="GC1">
+        <v>92</v>
+      </c>
+      <c r="GE1">
+        <v>93</v>
+      </c>
+      <c r="GG1">
+        <v>94</v>
+      </c>
+      <c r="GI1">
+        <v>95</v>
+      </c>
+      <c r="GK1">
+        <v>96</v>
+      </c>
+      <c r="GM1">
+        <v>97</v>
+      </c>
+      <c r="GO1">
+        <v>98</v>
+      </c>
+      <c r="GQ1">
+        <v>99</v>
+      </c>
+      <c r="GS1">
+        <v>100</v>
+      </c>
+      <c r="GU1">
+        <v>101</v>
+      </c>
+      <c r="GW1">
+        <v>102</v>
+      </c>
+      <c r="GY1">
+        <v>103</v>
+      </c>
+      <c r="HA1">
+        <v>104</v>
+      </c>
+      <c r="HC1">
+        <v>105</v>
+      </c>
+      <c r="HE1">
+        <v>106</v>
+      </c>
+      <c r="HG1">
+        <v>107</v>
+      </c>
+      <c r="HI1">
+        <v>108</v>
+      </c>
+      <c r="HK1">
+        <v>109</v>
+      </c>
+      <c r="HM1">
+        <v>110</v>
+      </c>
+      <c r="HO1">
+        <v>111</v>
+      </c>
+      <c r="HQ1">
+        <v>112</v>
+      </c>
+      <c r="HS1">
+        <v>113</v>
+      </c>
+      <c r="HU1">
+        <v>114</v>
+      </c>
+      <c r="HW1">
+        <v>115</v>
+      </c>
+      <c r="HY1">
+        <v>116</v>
+      </c>
+      <c r="IA1">
+        <v>117</v>
+      </c>
+      <c r="IC1">
+        <v>118</v>
+      </c>
+      <c r="IE1">
+        <v>119</v>
+      </c>
+      <c r="IG1">
+        <v>120</v>
+      </c>
+      <c r="II1">
+        <v>121</v>
+      </c>
+      <c r="IK1">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:245" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3386,8 +6052,185 @@
       <c r="DW2" t="s">
         <v>446</v>
       </c>
+      <c r="DY2" t="s">
+        <v>453</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>462</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>471</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>478</v>
+      </c>
+      <c r="EG2" t="s">
+        <v>485</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>491</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>498</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>504</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>511</v>
+      </c>
+      <c r="ES2" t="s">
+        <v>519</v>
+      </c>
+      <c r="EU2" t="s">
+        <v>526</v>
+      </c>
+      <c r="EW2" t="s">
+        <v>533</v>
+      </c>
+      <c r="EY2" t="s">
+        <v>540</v>
+      </c>
+      <c r="FA2" t="s">
+        <v>80</v>
+      </c>
+      <c r="FC2" t="s">
+        <v>547</v>
+      </c>
+      <c r="FE2" t="s">
+        <v>554</v>
+      </c>
+      <c r="FG2" t="s">
+        <v>561</v>
+      </c>
+      <c r="FI2" t="s">
+        <v>568</v>
+      </c>
+      <c r="FK2" t="s">
+        <v>575</v>
+      </c>
+      <c r="FM2" t="s">
+        <v>582</v>
+      </c>
+      <c r="FO2" t="s">
+        <v>589</v>
+      </c>
+      <c r="FQ2" t="s">
+        <v>596</v>
+      </c>
+      <c r="FS2" t="s">
+        <v>602</v>
+      </c>
+      <c r="FU2" t="s">
+        <v>609</v>
+      </c>
+      <c r="FW2" t="s">
+        <v>616</v>
+      </c>
+      <c r="FY2" t="s">
+        <v>623</v>
+      </c>
+      <c r="GA2" t="s">
+        <v>630</v>
+      </c>
+      <c r="GC2" t="s">
+        <v>636</v>
+      </c>
+      <c r="GE2" t="s">
+        <v>643</v>
+      </c>
+      <c r="GG2" t="s">
+        <v>650</v>
+      </c>
+      <c r="GI2" t="s">
+        <v>657</v>
+      </c>
+      <c r="GK2" t="s">
+        <v>663</v>
+      </c>
+      <c r="GM2" t="s">
+        <v>670</v>
+      </c>
+      <c r="GO2" t="s">
+        <v>677</v>
+      </c>
+      <c r="GQ2" t="s">
+        <v>684</v>
+      </c>
+      <c r="GS2" t="s">
+        <v>691</v>
+      </c>
+      <c r="GU2" t="s">
+        <v>697</v>
+      </c>
+      <c r="GW2" t="s">
+        <v>704</v>
+      </c>
+      <c r="GY2" t="s">
+        <v>345</v>
+      </c>
+      <c r="HA2" t="s">
+        <v>711</v>
+      </c>
+      <c r="HC2" t="s">
+        <v>718</v>
+      </c>
+      <c r="HE2" t="s">
+        <v>359</v>
+      </c>
+      <c r="HG2" t="s">
+        <v>725</v>
+      </c>
+      <c r="HI2" t="s">
+        <v>731</v>
+      </c>
+      <c r="HK2" t="s">
+        <v>738</v>
+      </c>
+      <c r="HM2" t="s">
+        <v>745</v>
+      </c>
+      <c r="HO2" t="s">
+        <v>752</v>
+      </c>
+      <c r="HQ2" t="s">
+        <v>378</v>
+      </c>
+      <c r="HS2" t="s">
+        <v>759</v>
+      </c>
+      <c r="HU2" t="s">
+        <v>767</v>
+      </c>
+      <c r="HW2" t="s">
+        <v>774</v>
+      </c>
+      <c r="HY2" t="s">
+        <v>781</v>
+      </c>
+      <c r="IA2" t="s">
+        <v>788</v>
+      </c>
+      <c r="IC2" t="s">
+        <v>794</v>
+      </c>
+      <c r="IE2" t="s">
+        <v>801</v>
+      </c>
+      <c r="IG2" t="s">
+        <v>807</v>
+      </c>
+      <c r="II2" t="s">
+        <v>813</v>
+      </c>
+      <c r="IK2" t="s">
+        <v>820</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:245" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3580,8 +6423,185 @@
       <c r="DW3" t="s">
         <v>447</v>
       </c>
+      <c r="DY3" t="s">
+        <v>454</v>
+      </c>
+      <c r="EA3" t="s">
+        <v>463</v>
+      </c>
+      <c r="EC3" t="s">
+        <v>472</v>
+      </c>
+      <c r="EE3" t="s">
+        <v>479</v>
+      </c>
+      <c r="EG3" t="s">
+        <v>486</v>
+      </c>
+      <c r="EI3" t="s">
+        <v>492</v>
+      </c>
+      <c r="EK3" t="s">
+        <v>37</v>
+      </c>
+      <c r="EM3" t="s">
+        <v>499</v>
+      </c>
+      <c r="EO3" t="s">
+        <v>505</v>
+      </c>
+      <c r="EQ3" t="s">
+        <v>512</v>
+      </c>
+      <c r="ES3" t="s">
+        <v>520</v>
+      </c>
+      <c r="EU3" t="s">
+        <v>527</v>
+      </c>
+      <c r="EW3" t="s">
+        <v>534</v>
+      </c>
+      <c r="EY3" t="s">
+        <v>541</v>
+      </c>
+      <c r="FA3" t="s">
+        <v>81</v>
+      </c>
+      <c r="FC3" t="s">
+        <v>548</v>
+      </c>
+      <c r="FE3" t="s">
+        <v>555</v>
+      </c>
+      <c r="FG3" t="s">
+        <v>562</v>
+      </c>
+      <c r="FI3" t="s">
+        <v>569</v>
+      </c>
+      <c r="FK3" t="s">
+        <v>576</v>
+      </c>
+      <c r="FM3" t="s">
+        <v>583</v>
+      </c>
+      <c r="FO3" t="s">
+        <v>590</v>
+      </c>
+      <c r="FQ3" t="s">
+        <v>597</v>
+      </c>
+      <c r="FS3" t="s">
+        <v>603</v>
+      </c>
+      <c r="FU3" t="s">
+        <v>610</v>
+      </c>
+      <c r="FW3" t="s">
+        <v>617</v>
+      </c>
+      <c r="FY3" t="s">
+        <v>624</v>
+      </c>
+      <c r="GA3" t="s">
+        <v>631</v>
+      </c>
+      <c r="GC3" t="s">
+        <v>637</v>
+      </c>
+      <c r="GE3" t="s">
+        <v>644</v>
+      </c>
+      <c r="GG3" t="s">
+        <v>651</v>
+      </c>
+      <c r="GI3" t="s">
+        <v>658</v>
+      </c>
+      <c r="GK3" t="s">
+        <v>664</v>
+      </c>
+      <c r="GM3" t="s">
+        <v>671</v>
+      </c>
+      <c r="GO3" t="s">
+        <v>678</v>
+      </c>
+      <c r="GQ3" t="s">
+        <v>685</v>
+      </c>
+      <c r="GS3" t="s">
+        <v>692</v>
+      </c>
+      <c r="GU3" t="s">
+        <v>698</v>
+      </c>
+      <c r="GW3" t="s">
+        <v>705</v>
+      </c>
+      <c r="GY3" t="s">
+        <v>346</v>
+      </c>
+      <c r="HA3" t="s">
+        <v>712</v>
+      </c>
+      <c r="HC3" t="s">
+        <v>719</v>
+      </c>
+      <c r="HE3" t="s">
+        <v>360</v>
+      </c>
+      <c r="HG3" t="s">
+        <v>726</v>
+      </c>
+      <c r="HI3" t="s">
+        <v>732</v>
+      </c>
+      <c r="HK3" t="s">
+        <v>739</v>
+      </c>
+      <c r="HM3" t="s">
+        <v>746</v>
+      </c>
+      <c r="HO3" t="s">
+        <v>753</v>
+      </c>
+      <c r="HQ3" t="s">
+        <v>379</v>
+      </c>
+      <c r="HS3" t="s">
+        <v>760</v>
+      </c>
+      <c r="HU3" t="s">
+        <v>768</v>
+      </c>
+      <c r="HW3" t="s">
+        <v>775</v>
+      </c>
+      <c r="HY3" t="s">
+        <v>782</v>
+      </c>
+      <c r="IA3" t="s">
+        <v>789</v>
+      </c>
+      <c r="IC3" t="s">
+        <v>795</v>
+      </c>
+      <c r="IE3" t="s">
+        <v>802</v>
+      </c>
+      <c r="IG3" t="s">
+        <v>808</v>
+      </c>
+      <c r="II3" t="s">
+        <v>814</v>
+      </c>
+      <c r="IK3" t="s">
+        <v>821</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:245" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -3774,8 +6794,185 @@
       <c r="DW4" t="s">
         <v>448</v>
       </c>
+      <c r="DY4" t="s">
+        <v>455</v>
+      </c>
+      <c r="EA4" t="s">
+        <v>464</v>
+      </c>
+      <c r="EC4" t="s">
+        <v>473</v>
+      </c>
+      <c r="EE4" t="s">
+        <v>480</v>
+      </c>
+      <c r="EG4" t="s">
+        <v>126</v>
+      </c>
+      <c r="EI4" t="s">
+        <v>493</v>
+      </c>
+      <c r="EK4" t="s">
+        <v>38</v>
+      </c>
+      <c r="EM4" t="s">
+        <v>428</v>
+      </c>
+      <c r="EO4" t="s">
+        <v>506</v>
+      </c>
+      <c r="EQ4" t="s">
+        <v>513</v>
+      </c>
+      <c r="ES4" t="s">
+        <v>521</v>
+      </c>
+      <c r="EU4" t="s">
+        <v>528</v>
+      </c>
+      <c r="EW4" t="s">
+        <v>535</v>
+      </c>
+      <c r="EY4" t="s">
+        <v>542</v>
+      </c>
+      <c r="FA4" t="s">
+        <v>82</v>
+      </c>
+      <c r="FC4" t="s">
+        <v>549</v>
+      </c>
+      <c r="FE4" t="s">
+        <v>45</v>
+      </c>
+      <c r="FG4" t="s">
+        <v>563</v>
+      </c>
+      <c r="FI4" t="s">
+        <v>570</v>
+      </c>
+      <c r="FK4" t="s">
+        <v>577</v>
+      </c>
+      <c r="FM4" t="s">
+        <v>584</v>
+      </c>
+      <c r="FO4" t="s">
+        <v>591</v>
+      </c>
+      <c r="FQ4" t="s">
+        <v>126</v>
+      </c>
+      <c r="FS4" t="s">
+        <v>387</v>
+      </c>
+      <c r="FU4" t="s">
+        <v>611</v>
+      </c>
+      <c r="FW4" t="s">
+        <v>618</v>
+      </c>
+      <c r="FY4" t="s">
+        <v>625</v>
+      </c>
+      <c r="GA4" t="s">
+        <v>591</v>
+      </c>
+      <c r="GC4" t="s">
+        <v>638</v>
+      </c>
+      <c r="GE4" t="s">
+        <v>645</v>
+      </c>
+      <c r="GG4" t="s">
+        <v>652</v>
+      </c>
+      <c r="GI4" t="s">
+        <v>314</v>
+      </c>
+      <c r="GK4" t="s">
+        <v>665</v>
+      </c>
+      <c r="GM4" t="s">
+        <v>672</v>
+      </c>
+      <c r="GO4" t="s">
+        <v>679</v>
+      </c>
+      <c r="GQ4" t="s">
+        <v>686</v>
+      </c>
+      <c r="GS4" t="s">
+        <v>672</v>
+      </c>
+      <c r="GU4" t="s">
+        <v>699</v>
+      </c>
+      <c r="GW4" t="s">
+        <v>706</v>
+      </c>
+      <c r="GY4" t="s">
+        <v>347</v>
+      </c>
+      <c r="HA4" t="s">
+        <v>713</v>
+      </c>
+      <c r="HC4" t="s">
+        <v>720</v>
+      </c>
+      <c r="HE4" t="s">
+        <v>170</v>
+      </c>
+      <c r="HG4" t="s">
+        <v>149</v>
+      </c>
+      <c r="HI4" t="s">
+        <v>733</v>
+      </c>
+      <c r="HK4" t="s">
+        <v>740</v>
+      </c>
+      <c r="HM4" t="s">
+        <v>747</v>
+      </c>
+      <c r="HO4" t="s">
+        <v>754</v>
+      </c>
+      <c r="HQ4" t="s">
+        <v>380</v>
+      </c>
+      <c r="HS4" t="s">
+        <v>761</v>
+      </c>
+      <c r="HU4" t="s">
+        <v>769</v>
+      </c>
+      <c r="HW4" t="s">
+        <v>776</v>
+      </c>
+      <c r="HY4" t="s">
+        <v>783</v>
+      </c>
+      <c r="IA4" t="s">
+        <v>618</v>
+      </c>
+      <c r="IC4" t="s">
+        <v>796</v>
+      </c>
+      <c r="IE4" t="s">
+        <v>713</v>
+      </c>
+      <c r="IG4" t="s">
+        <v>591</v>
+      </c>
+      <c r="II4" t="s">
+        <v>815</v>
+      </c>
+      <c r="IK4" t="s">
+        <v>706</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:245" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -3968,8 +7165,185 @@
       <c r="DW5" t="s">
         <v>449</v>
       </c>
+      <c r="DY5" t="s">
+        <v>456</v>
+      </c>
+      <c r="EA5" t="s">
+        <v>465</v>
+      </c>
+      <c r="EC5" t="s">
+        <v>474</v>
+      </c>
+      <c r="EE5" t="s">
+        <v>481</v>
+      </c>
+      <c r="EG5" t="s">
+        <v>487</v>
+      </c>
+      <c r="EI5" t="s">
+        <v>494</v>
+      </c>
+      <c r="EK5" t="s">
+        <v>39</v>
+      </c>
+      <c r="EM5" t="s">
+        <v>500</v>
+      </c>
+      <c r="EO5" t="s">
+        <v>507</v>
+      </c>
+      <c r="EQ5" t="s">
+        <v>514</v>
+      </c>
+      <c r="ES5" t="s">
+        <v>522</v>
+      </c>
+      <c r="EU5" t="s">
+        <v>529</v>
+      </c>
+      <c r="EW5" t="s">
+        <v>536</v>
+      </c>
+      <c r="EY5" t="s">
+        <v>543</v>
+      </c>
+      <c r="FA5" t="s">
+        <v>83</v>
+      </c>
+      <c r="FC5" t="s">
+        <v>550</v>
+      </c>
+      <c r="FE5" t="s">
+        <v>556</v>
+      </c>
+      <c r="FG5" t="s">
+        <v>564</v>
+      </c>
+      <c r="FI5" t="s">
+        <v>571</v>
+      </c>
+      <c r="FK5" t="s">
+        <v>578</v>
+      </c>
+      <c r="FM5" t="s">
+        <v>585</v>
+      </c>
+      <c r="FO5" t="s">
+        <v>592</v>
+      </c>
+      <c r="FQ5" t="s">
+        <v>598</v>
+      </c>
+      <c r="FS5" t="s">
+        <v>604</v>
+      </c>
+      <c r="FU5" t="s">
+        <v>612</v>
+      </c>
+      <c r="FW5" t="s">
+        <v>619</v>
+      </c>
+      <c r="FY5" t="s">
+        <v>626</v>
+      </c>
+      <c r="GA5" t="s">
+        <v>632</v>
+      </c>
+      <c r="GC5" t="s">
+        <v>639</v>
+      </c>
+      <c r="GE5" t="s">
+        <v>646</v>
+      </c>
+      <c r="GG5" t="s">
+        <v>653</v>
+      </c>
+      <c r="GI5" t="s">
+        <v>659</v>
+      </c>
+      <c r="GK5" t="s">
+        <v>666</v>
+      </c>
+      <c r="GM5" t="s">
+        <v>673</v>
+      </c>
+      <c r="GO5" t="s">
+        <v>680</v>
+      </c>
+      <c r="GQ5" t="s">
+        <v>687</v>
+      </c>
+      <c r="GS5" t="s">
+        <v>693</v>
+      </c>
+      <c r="GU5" t="s">
+        <v>700</v>
+      </c>
+      <c r="GW5" t="s">
+        <v>707</v>
+      </c>
+      <c r="GY5" t="s">
+        <v>348</v>
+      </c>
+      <c r="HA5" t="s">
+        <v>714</v>
+      </c>
+      <c r="HC5" t="s">
+        <v>721</v>
+      </c>
+      <c r="HE5" t="s">
+        <v>361</v>
+      </c>
+      <c r="HG5" t="s">
+        <v>727</v>
+      </c>
+      <c r="HI5" t="s">
+        <v>734</v>
+      </c>
+      <c r="HK5" t="s">
+        <v>741</v>
+      </c>
+      <c r="HM5" t="s">
+        <v>748</v>
+      </c>
+      <c r="HO5" t="s">
+        <v>755</v>
+      </c>
+      <c r="HQ5" t="s">
+        <v>381</v>
+      </c>
+      <c r="HS5" t="s">
+        <v>762</v>
+      </c>
+      <c r="HU5" t="s">
+        <v>770</v>
+      </c>
+      <c r="HW5" t="s">
+        <v>777</v>
+      </c>
+      <c r="HY5" t="s">
+        <v>784</v>
+      </c>
+      <c r="IA5" t="s">
+        <v>790</v>
+      </c>
+      <c r="IC5" t="s">
+        <v>797</v>
+      </c>
+      <c r="IE5" t="s">
+        <v>803</v>
+      </c>
+      <c r="IG5" t="s">
+        <v>809</v>
+      </c>
+      <c r="II5" t="s">
+        <v>816</v>
+      </c>
+      <c r="IK5" t="s">
+        <v>822</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:245" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4162,8 +7536,185 @@
       <c r="DW6" t="s">
         <v>24</v>
       </c>
+      <c r="DY6" t="s">
+        <v>32</v>
+      </c>
+      <c r="EA6" t="s">
+        <v>466</v>
+      </c>
+      <c r="EC6" t="s">
+        <v>32</v>
+      </c>
+      <c r="EE6" t="s">
+        <v>32</v>
+      </c>
+      <c r="EG6" t="s">
+        <v>14</v>
+      </c>
+      <c r="EI6" t="s">
+        <v>14</v>
+      </c>
+      <c r="EK6" t="s">
+        <v>24</v>
+      </c>
+      <c r="EM6" t="s">
+        <v>14</v>
+      </c>
+      <c r="EO6" t="s">
+        <v>47</v>
+      </c>
+      <c r="EQ6" t="s">
+        <v>32</v>
+      </c>
+      <c r="ES6" t="s">
+        <v>24</v>
+      </c>
+      <c r="EU6" t="s">
+        <v>14</v>
+      </c>
+      <c r="EW6" t="s">
+        <v>32</v>
+      </c>
+      <c r="EY6" t="s">
+        <v>32</v>
+      </c>
+      <c r="FA6" t="s">
+        <v>84</v>
+      </c>
+      <c r="FC6" t="s">
+        <v>32</v>
+      </c>
+      <c r="FE6" t="s">
+        <v>14</v>
+      </c>
+      <c r="FG6" t="s">
+        <v>14</v>
+      </c>
+      <c r="FI6" t="s">
+        <v>47</v>
+      </c>
+      <c r="FK6" t="s">
+        <v>32</v>
+      </c>
+      <c r="FM6" t="s">
+        <v>14</v>
+      </c>
+      <c r="FO6" t="s">
+        <v>164</v>
+      </c>
+      <c r="FQ6" t="s">
+        <v>32</v>
+      </c>
+      <c r="FS6" t="s">
+        <v>47</v>
+      </c>
+      <c r="FU6" t="s">
+        <v>14</v>
+      </c>
+      <c r="FW6" t="s">
+        <v>14</v>
+      </c>
+      <c r="FY6" t="s">
+        <v>32</v>
+      </c>
+      <c r="GA6" t="s">
+        <v>47</v>
+      </c>
+      <c r="GC6" t="s">
+        <v>47</v>
+      </c>
+      <c r="GE6" t="s">
+        <v>14</v>
+      </c>
+      <c r="GG6" t="s">
+        <v>32</v>
+      </c>
+      <c r="GI6" t="s">
+        <v>32</v>
+      </c>
+      <c r="GK6" t="s">
+        <v>14</v>
+      </c>
+      <c r="GM6" t="s">
+        <v>32</v>
+      </c>
+      <c r="GO6" t="s">
+        <v>14</v>
+      </c>
+      <c r="GQ6" t="s">
+        <v>14</v>
+      </c>
+      <c r="GS6" t="s">
+        <v>47</v>
+      </c>
+      <c r="GU6" t="s">
+        <v>14</v>
+      </c>
+      <c r="GW6" t="s">
+        <v>14</v>
+      </c>
+      <c r="GY6" t="s">
+        <v>84</v>
+      </c>
+      <c r="HA6" t="s">
+        <v>47</v>
+      </c>
+      <c r="HC6" t="s">
+        <v>14</v>
+      </c>
+      <c r="HE6" t="s">
+        <v>14</v>
+      </c>
+      <c r="HG6" t="s">
+        <v>47</v>
+      </c>
+      <c r="HI6" t="s">
+        <v>14</v>
+      </c>
+      <c r="HK6" t="s">
+        <v>32</v>
+      </c>
+      <c r="HM6" t="s">
+        <v>14</v>
+      </c>
+      <c r="HO6" t="s">
+        <v>14</v>
+      </c>
+      <c r="HQ6" t="s">
+        <v>32</v>
+      </c>
+      <c r="HS6" t="s">
+        <v>14</v>
+      </c>
+      <c r="HU6" t="s">
+        <v>32</v>
+      </c>
+      <c r="HW6" t="s">
+        <v>32</v>
+      </c>
+      <c r="HY6" t="s">
+        <v>32</v>
+      </c>
+      <c r="IA6" t="s">
+        <v>32</v>
+      </c>
+      <c r="IC6" t="s">
+        <v>84</v>
+      </c>
+      <c r="IE6" t="s">
+        <v>14</v>
+      </c>
+      <c r="IG6" t="s">
+        <v>47</v>
+      </c>
+      <c r="II6" t="s">
+        <v>32</v>
+      </c>
+      <c r="IK6" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:245" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -4356,8 +7907,185 @@
       <c r="DW7" t="s">
         <v>70</v>
       </c>
+      <c r="DY7" t="s">
+        <v>457</v>
+      </c>
+      <c r="EA7" t="s">
+        <v>467</v>
+      </c>
+      <c r="EC7" t="s">
+        <v>99</v>
+      </c>
+      <c r="EE7" t="s">
+        <v>355</v>
+      </c>
+      <c r="EG7" t="s">
+        <v>84</v>
+      </c>
+      <c r="EI7" t="s">
+        <v>295</v>
+      </c>
+      <c r="EK7" t="s">
+        <v>32</v>
+      </c>
+      <c r="EM7" t="s">
+        <v>295</v>
+      </c>
+      <c r="EO7" t="s">
+        <v>84</v>
+      </c>
+      <c r="EQ7" t="s">
+        <v>515</v>
+      </c>
+      <c r="ES7" t="s">
+        <v>84</v>
+      </c>
+      <c r="EU7" t="s">
+        <v>70</v>
+      </c>
+      <c r="EW7" t="s">
+        <v>84</v>
+      </c>
+      <c r="EY7" t="s">
+        <v>84</v>
+      </c>
+      <c r="FA7" t="s">
+        <v>84</v>
+      </c>
+      <c r="FC7" t="s">
+        <v>32</v>
+      </c>
+      <c r="FE7" t="s">
+        <v>557</v>
+      </c>
+      <c r="FG7" t="s">
+        <v>15</v>
+      </c>
+      <c r="FI7" t="s">
+        <v>70</v>
+      </c>
+      <c r="FK7" t="s">
+        <v>47</v>
+      </c>
+      <c r="FM7" t="s">
+        <v>70</v>
+      </c>
+      <c r="FO7" t="s">
+        <v>32</v>
+      </c>
+      <c r="FQ7" t="s">
+        <v>70</v>
+      </c>
+      <c r="FS7" t="s">
+        <v>605</v>
+      </c>
+      <c r="FU7" t="s">
+        <v>295</v>
+      </c>
+      <c r="FW7" t="s">
+        <v>84</v>
+      </c>
+      <c r="FY7" t="s">
+        <v>143</v>
+      </c>
+      <c r="GA7" t="s">
+        <v>32</v>
+      </c>
+      <c r="GC7" t="s">
+        <v>70</v>
+      </c>
+      <c r="GE7" t="s">
+        <v>70</v>
+      </c>
+      <c r="GG7" t="s">
+        <v>70</v>
+      </c>
+      <c r="GI7" t="s">
+        <v>70</v>
+      </c>
+      <c r="GK7" t="s">
+        <v>14</v>
+      </c>
+      <c r="GM7" t="s">
+        <v>32</v>
+      </c>
+      <c r="GO7" t="s">
+        <v>32</v>
+      </c>
+      <c r="GQ7" t="s">
+        <v>32</v>
+      </c>
+      <c r="GS7" t="s">
+        <v>295</v>
+      </c>
+      <c r="GU7" t="s">
+        <v>70</v>
+      </c>
+      <c r="GW7" t="s">
+        <v>143</v>
+      </c>
+      <c r="GY7" t="s">
+        <v>295</v>
+      </c>
+      <c r="HA7" t="s">
+        <v>70</v>
+      </c>
+      <c r="HC7" t="s">
+        <v>70</v>
+      </c>
+      <c r="HE7" t="s">
+        <v>128</v>
+      </c>
+      <c r="HG7" t="s">
+        <v>70</v>
+      </c>
+      <c r="HI7" t="s">
+        <v>70</v>
+      </c>
+      <c r="HK7" t="s">
+        <v>605</v>
+      </c>
+      <c r="HM7" t="s">
+        <v>70</v>
+      </c>
+      <c r="HO7" t="s">
+        <v>515</v>
+      </c>
+      <c r="HQ7" t="s">
+        <v>14</v>
+      </c>
+      <c r="HS7" t="s">
+        <v>763</v>
+      </c>
+      <c r="HU7" t="s">
+        <v>70</v>
+      </c>
+      <c r="HW7" t="s">
+        <v>14</v>
+      </c>
+      <c r="HY7" t="s">
+        <v>763</v>
+      </c>
+      <c r="IA7" t="s">
+        <v>70</v>
+      </c>
+      <c r="IC7" t="s">
+        <v>70</v>
+      </c>
+      <c r="IE7" t="s">
+        <v>70</v>
+      </c>
+      <c r="IG7" t="s">
+        <v>70</v>
+      </c>
+      <c r="II7" t="s">
+        <v>70</v>
+      </c>
+      <c r="IK7" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:245" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -4550,8 +8278,185 @@
       <c r="DW8" t="s">
         <v>450</v>
       </c>
+      <c r="DY8" t="s">
+        <v>458</v>
+      </c>
+      <c r="EA8" t="s">
+        <v>468</v>
+      </c>
+      <c r="EC8" t="s">
+        <v>475</v>
+      </c>
+      <c r="EE8" t="s">
+        <v>482</v>
+      </c>
+      <c r="EG8" t="s">
+        <v>488</v>
+      </c>
+      <c r="EI8" t="s">
+        <v>495</v>
+      </c>
+      <c r="EK8" t="s">
+        <v>40</v>
+      </c>
+      <c r="EM8" t="s">
+        <v>501</v>
+      </c>
+      <c r="EO8" t="s">
+        <v>508</v>
+      </c>
+      <c r="EQ8" t="s">
+        <v>516</v>
+      </c>
+      <c r="ES8" t="s">
+        <v>523</v>
+      </c>
+      <c r="EU8" t="s">
+        <v>530</v>
+      </c>
+      <c r="EW8" t="s">
+        <v>537</v>
+      </c>
+      <c r="EY8" t="s">
+        <v>544</v>
+      </c>
+      <c r="FA8" t="s">
+        <v>85</v>
+      </c>
+      <c r="FC8" t="s">
+        <v>551</v>
+      </c>
+      <c r="FE8" t="s">
+        <v>558</v>
+      </c>
+      <c r="FG8" t="s">
+        <v>565</v>
+      </c>
+      <c r="FI8" t="s">
+        <v>572</v>
+      </c>
+      <c r="FK8" t="s">
+        <v>579</v>
+      </c>
+      <c r="FM8" t="s">
+        <v>586</v>
+      </c>
+      <c r="FO8" t="s">
+        <v>593</v>
+      </c>
+      <c r="FQ8" t="s">
+        <v>599</v>
+      </c>
+      <c r="FS8" t="s">
+        <v>606</v>
+      </c>
+      <c r="FU8" t="s">
+        <v>613</v>
+      </c>
+      <c r="FW8" t="s">
+        <v>620</v>
+      </c>
+      <c r="FY8" t="s">
+        <v>627</v>
+      </c>
+      <c r="GA8" t="s">
+        <v>633</v>
+      </c>
+      <c r="GC8" t="s">
+        <v>640</v>
+      </c>
+      <c r="GE8" t="s">
+        <v>647</v>
+      </c>
+      <c r="GG8" t="s">
+        <v>654</v>
+      </c>
+      <c r="GI8" t="s">
+        <v>660</v>
+      </c>
+      <c r="GK8" t="s">
+        <v>667</v>
+      </c>
+      <c r="GM8" t="s">
+        <v>674</v>
+      </c>
+      <c r="GO8" t="s">
+        <v>681</v>
+      </c>
+      <c r="GQ8" t="s">
+        <v>688</v>
+      </c>
+      <c r="GS8" t="s">
+        <v>694</v>
+      </c>
+      <c r="GU8" t="s">
+        <v>701</v>
+      </c>
+      <c r="GW8" t="s">
+        <v>708</v>
+      </c>
+      <c r="GY8" t="s">
+        <v>349</v>
+      </c>
+      <c r="HA8" t="s">
+        <v>715</v>
+      </c>
+      <c r="HC8" t="s">
+        <v>722</v>
+      </c>
+      <c r="HE8" t="s">
+        <v>362</v>
+      </c>
+      <c r="HG8" t="s">
+        <v>728</v>
+      </c>
+      <c r="HI8" t="s">
+        <v>735</v>
+      </c>
+      <c r="HK8" t="s">
+        <v>742</v>
+      </c>
+      <c r="HM8" t="s">
+        <v>749</v>
+      </c>
+      <c r="HO8" t="s">
+        <v>756</v>
+      </c>
+      <c r="HQ8" t="s">
+        <v>382</v>
+      </c>
+      <c r="HS8" t="s">
+        <v>764</v>
+      </c>
+      <c r="HU8" t="s">
+        <v>771</v>
+      </c>
+      <c r="HW8" t="s">
+        <v>778</v>
+      </c>
+      <c r="HY8" t="s">
+        <v>785</v>
+      </c>
+      <c r="IA8" t="s">
+        <v>791</v>
+      </c>
+      <c r="IC8" t="s">
+        <v>798</v>
+      </c>
+      <c r="IE8" t="s">
+        <v>804</v>
+      </c>
+      <c r="IG8" t="s">
+        <v>810</v>
+      </c>
+      <c r="II8" t="s">
+        <v>817</v>
+      </c>
+      <c r="IK8" t="s">
+        <v>823</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:245" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -4744,8 +8649,185 @@
       <c r="DW9" t="s">
         <v>451</v>
       </c>
+      <c r="DY9" t="s">
+        <v>459</v>
+      </c>
+      <c r="EA9" t="s">
+        <v>469</v>
+      </c>
+      <c r="EC9" t="s">
+        <v>476</v>
+      </c>
+      <c r="EE9" t="s">
+        <v>483</v>
+      </c>
+      <c r="EG9" t="s">
+        <v>489</v>
+      </c>
+      <c r="EI9" t="s">
+        <v>496</v>
+      </c>
+      <c r="EK9" t="s">
+        <v>41</v>
+      </c>
+      <c r="EM9" t="s">
+        <v>502</v>
+      </c>
+      <c r="EO9" t="s">
+        <v>509</v>
+      </c>
+      <c r="EQ9" t="s">
+        <v>517</v>
+      </c>
+      <c r="ES9" t="s">
+        <v>524</v>
+      </c>
+      <c r="EU9" t="s">
+        <v>531</v>
+      </c>
+      <c r="EW9" t="s">
+        <v>538</v>
+      </c>
+      <c r="EY9" t="s">
+        <v>545</v>
+      </c>
+      <c r="FA9" t="s">
+        <v>86</v>
+      </c>
+      <c r="FC9" t="s">
+        <v>552</v>
+      </c>
+      <c r="FE9" t="s">
+        <v>559</v>
+      </c>
+      <c r="FG9" t="s">
+        <v>566</v>
+      </c>
+      <c r="FI9" t="s">
+        <v>573</v>
+      </c>
+      <c r="FK9" t="s">
+        <v>580</v>
+      </c>
+      <c r="FM9" t="s">
+        <v>587</v>
+      </c>
+      <c r="FO9" t="s">
+        <v>594</v>
+      </c>
+      <c r="FQ9" t="s">
+        <v>600</v>
+      </c>
+      <c r="FS9" t="s">
+        <v>607</v>
+      </c>
+      <c r="FU9" t="s">
+        <v>614</v>
+      </c>
+      <c r="FW9" t="s">
+        <v>621</v>
+      </c>
+      <c r="FY9" t="s">
+        <v>628</v>
+      </c>
+      <c r="GA9" t="s">
+        <v>634</v>
+      </c>
+      <c r="GC9" t="s">
+        <v>641</v>
+      </c>
+      <c r="GE9" t="s">
+        <v>648</v>
+      </c>
+      <c r="GG9" t="s">
+        <v>655</v>
+      </c>
+      <c r="GI9" t="s">
+        <v>661</v>
+      </c>
+      <c r="GK9" t="s">
+        <v>668</v>
+      </c>
+      <c r="GM9" t="s">
+        <v>675</v>
+      </c>
+      <c r="GO9" t="s">
+        <v>682</v>
+      </c>
+      <c r="GQ9" t="s">
+        <v>689</v>
+      </c>
+      <c r="GS9" t="s">
+        <v>695</v>
+      </c>
+      <c r="GU9" t="s">
+        <v>702</v>
+      </c>
+      <c r="GW9" t="s">
+        <v>709</v>
+      </c>
+      <c r="GY9" t="s">
+        <v>350</v>
+      </c>
+      <c r="HA9" t="s">
+        <v>716</v>
+      </c>
+      <c r="HC9" t="s">
+        <v>723</v>
+      </c>
+      <c r="HE9" t="s">
+        <v>363</v>
+      </c>
+      <c r="HG9" t="s">
+        <v>729</v>
+      </c>
+      <c r="HI9" t="s">
+        <v>736</v>
+      </c>
+      <c r="HK9" t="s">
+        <v>743</v>
+      </c>
+      <c r="HM9" t="s">
+        <v>750</v>
+      </c>
+      <c r="HO9" t="s">
+        <v>757</v>
+      </c>
+      <c r="HQ9" t="s">
+        <v>383</v>
+      </c>
+      <c r="HS9" t="s">
+        <v>765</v>
+      </c>
+      <c r="HU9" t="s">
+        <v>772</v>
+      </c>
+      <c r="HW9" t="s">
+        <v>779</v>
+      </c>
+      <c r="HY9" t="s">
+        <v>786</v>
+      </c>
+      <c r="IA9" t="s">
+        <v>792</v>
+      </c>
+      <c r="IC9" t="s">
+        <v>799</v>
+      </c>
+      <c r="IE9" t="s">
+        <v>805</v>
+      </c>
+      <c r="IG9" t="s">
+        <v>811</v>
+      </c>
+      <c r="II9" t="s">
+        <v>818</v>
+      </c>
+      <c r="IK9" t="s">
+        <v>824</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:245" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -4938,8 +9020,185 @@
       <c r="DW10" t="s">
         <v>18</v>
       </c>
+      <c r="DY10" t="s">
+        <v>460</v>
+      </c>
+      <c r="EA10" t="s">
+        <v>460</v>
+      </c>
+      <c r="EC10" t="s">
+        <v>460</v>
+      </c>
+      <c r="EE10" t="s">
+        <v>460</v>
+      </c>
+      <c r="EG10" t="s">
+        <v>460</v>
+      </c>
+      <c r="EI10" t="s">
+        <v>460</v>
+      </c>
+      <c r="EK10" t="s">
+        <v>460</v>
+      </c>
+      <c r="EM10" t="s">
+        <v>460</v>
+      </c>
+      <c r="EO10" t="s">
+        <v>460</v>
+      </c>
+      <c r="EQ10" t="s">
+        <v>460</v>
+      </c>
+      <c r="ES10" t="s">
+        <v>460</v>
+      </c>
+      <c r="EU10" t="s">
+        <v>460</v>
+      </c>
+      <c r="EW10" t="s">
+        <v>460</v>
+      </c>
+      <c r="EY10" t="s">
+        <v>460</v>
+      </c>
+      <c r="FA10" t="s">
+        <v>460</v>
+      </c>
+      <c r="FC10" t="s">
+        <v>460</v>
+      </c>
+      <c r="FE10" t="s">
+        <v>460</v>
+      </c>
+      <c r="FG10" t="s">
+        <v>460</v>
+      </c>
+      <c r="FI10" t="s">
+        <v>460</v>
+      </c>
+      <c r="FK10" t="s">
+        <v>460</v>
+      </c>
+      <c r="FM10" t="s">
+        <v>460</v>
+      </c>
+      <c r="FO10" t="s">
+        <v>460</v>
+      </c>
+      <c r="FQ10" t="s">
+        <v>460</v>
+      </c>
+      <c r="FS10" t="s">
+        <v>460</v>
+      </c>
+      <c r="FU10" t="s">
+        <v>460</v>
+      </c>
+      <c r="FW10" t="s">
+        <v>460</v>
+      </c>
+      <c r="FY10" t="s">
+        <v>460</v>
+      </c>
+      <c r="GA10" t="s">
+        <v>460</v>
+      </c>
+      <c r="GC10" t="s">
+        <v>460</v>
+      </c>
+      <c r="GE10" t="s">
+        <v>460</v>
+      </c>
+      <c r="GG10" t="s">
+        <v>460</v>
+      </c>
+      <c r="GI10" t="s">
+        <v>460</v>
+      </c>
+      <c r="GK10" t="s">
+        <v>460</v>
+      </c>
+      <c r="GM10" t="s">
+        <v>460</v>
+      </c>
+      <c r="GO10" t="s">
+        <v>460</v>
+      </c>
+      <c r="GQ10" t="s">
+        <v>460</v>
+      </c>
+      <c r="GS10" t="s">
+        <v>460</v>
+      </c>
+      <c r="GU10" t="s">
+        <v>460</v>
+      </c>
+      <c r="GW10" t="s">
+        <v>460</v>
+      </c>
+      <c r="GY10" t="s">
+        <v>460</v>
+      </c>
+      <c r="HA10" t="s">
+        <v>460</v>
+      </c>
+      <c r="HC10" t="s">
+        <v>460</v>
+      </c>
+      <c r="HE10" t="s">
+        <v>460</v>
+      </c>
+      <c r="HG10" t="s">
+        <v>460</v>
+      </c>
+      <c r="HI10" t="s">
+        <v>460</v>
+      </c>
+      <c r="HK10" t="s">
+        <v>460</v>
+      </c>
+      <c r="HM10" t="s">
+        <v>460</v>
+      </c>
+      <c r="HO10" t="s">
+        <v>460</v>
+      </c>
+      <c r="HQ10" t="s">
+        <v>460</v>
+      </c>
+      <c r="HS10" t="s">
+        <v>460</v>
+      </c>
+      <c r="HU10" t="s">
+        <v>460</v>
+      </c>
+      <c r="HW10" t="s">
+        <v>460</v>
+      </c>
+      <c r="HY10" t="s">
+        <v>460</v>
+      </c>
+      <c r="IA10" t="s">
+        <v>460</v>
+      </c>
+      <c r="IC10" t="s">
+        <v>460</v>
+      </c>
+      <c r="IE10" t="s">
+        <v>460</v>
+      </c>
+      <c r="IG10" t="s">
+        <v>460</v>
+      </c>
+      <c r="II10" t="s">
+        <v>460</v>
+      </c>
+      <c r="IK10" t="s">
+        <v>460</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:245" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -5131,6 +9390,183 @@
       </c>
       <c r="DW11" t="s">
         <v>452</v>
+      </c>
+      <c r="DY11" t="s">
+        <v>461</v>
+      </c>
+      <c r="EA11" t="s">
+        <v>470</v>
+      </c>
+      <c r="EC11" t="s">
+        <v>477</v>
+      </c>
+      <c r="EE11" t="s">
+        <v>484</v>
+      </c>
+      <c r="EG11" t="s">
+        <v>490</v>
+      </c>
+      <c r="EI11" t="s">
+        <v>497</v>
+      </c>
+      <c r="EK11" t="s">
+        <v>42</v>
+      </c>
+      <c r="EM11" t="s">
+        <v>503</v>
+      </c>
+      <c r="EO11" t="s">
+        <v>510</v>
+      </c>
+      <c r="EQ11" t="s">
+        <v>518</v>
+      </c>
+      <c r="ES11" t="s">
+        <v>525</v>
+      </c>
+      <c r="EU11" t="s">
+        <v>532</v>
+      </c>
+      <c r="EW11" t="s">
+        <v>539</v>
+      </c>
+      <c r="EY11" t="s">
+        <v>546</v>
+      </c>
+      <c r="FA11" t="s">
+        <v>87</v>
+      </c>
+      <c r="FC11" t="s">
+        <v>553</v>
+      </c>
+      <c r="FE11" t="s">
+        <v>560</v>
+      </c>
+      <c r="FG11" t="s">
+        <v>567</v>
+      </c>
+      <c r="FI11" t="s">
+        <v>574</v>
+      </c>
+      <c r="FK11" t="s">
+        <v>581</v>
+      </c>
+      <c r="FM11" t="s">
+        <v>588</v>
+      </c>
+      <c r="FO11" t="s">
+        <v>595</v>
+      </c>
+      <c r="FQ11" t="s">
+        <v>601</v>
+      </c>
+      <c r="FS11" t="s">
+        <v>608</v>
+      </c>
+      <c r="FU11" t="s">
+        <v>615</v>
+      </c>
+      <c r="FW11" t="s">
+        <v>622</v>
+      </c>
+      <c r="FY11" t="s">
+        <v>629</v>
+      </c>
+      <c r="GA11" t="s">
+        <v>635</v>
+      </c>
+      <c r="GC11" t="s">
+        <v>642</v>
+      </c>
+      <c r="GE11" t="s">
+        <v>649</v>
+      </c>
+      <c r="GG11" t="s">
+        <v>656</v>
+      </c>
+      <c r="GI11" t="s">
+        <v>662</v>
+      </c>
+      <c r="GK11" t="s">
+        <v>669</v>
+      </c>
+      <c r="GM11" t="s">
+        <v>676</v>
+      </c>
+      <c r="GO11" t="s">
+        <v>683</v>
+      </c>
+      <c r="GQ11" t="s">
+        <v>690</v>
+      </c>
+      <c r="GS11" t="s">
+        <v>696</v>
+      </c>
+      <c r="GU11" t="s">
+        <v>703</v>
+      </c>
+      <c r="GW11" t="s">
+        <v>710</v>
+      </c>
+      <c r="GY11" t="s">
+        <v>351</v>
+      </c>
+      <c r="HA11" t="s">
+        <v>717</v>
+      </c>
+      <c r="HC11" t="s">
+        <v>724</v>
+      </c>
+      <c r="HE11" t="s">
+        <v>364</v>
+      </c>
+      <c r="HG11" t="s">
+        <v>730</v>
+      </c>
+      <c r="HI11" t="s">
+        <v>737</v>
+      </c>
+      <c r="HK11" t="s">
+        <v>744</v>
+      </c>
+      <c r="HM11" t="s">
+        <v>751</v>
+      </c>
+      <c r="HO11" t="s">
+        <v>758</v>
+      </c>
+      <c r="HQ11" t="s">
+        <v>384</v>
+      </c>
+      <c r="HS11" t="s">
+        <v>766</v>
+      </c>
+      <c r="HU11" t="s">
+        <v>773</v>
+      </c>
+      <c r="HW11" t="s">
+        <v>780</v>
+      </c>
+      <c r="HY11" t="s">
+        <v>787</v>
+      </c>
+      <c r="IA11" t="s">
+        <v>793</v>
+      </c>
+      <c r="IC11" t="s">
+        <v>800</v>
+      </c>
+      <c r="IE11" t="s">
+        <v>806</v>
+      </c>
+      <c r="IG11" t="s">
+        <v>812</v>
+      </c>
+      <c r="II11" t="s">
+        <v>819</v>
+      </c>
+      <c r="IK11" t="s">
+        <v>825</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final commit code-Recipe Scraping 2023
</commit_message>
<xml_diff>
--- a/Team02_NinjaScrapers_2023/src/test/resources/AllergyRecipes.xlsx
+++ b/Team02_NinjaScrapers_2023/src/test/resources/AllergyRecipes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akash\git\RecipeScrapingHackathon2023\Team02_NinjaScrapers_2023\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BDAFE2-E44F-424C-AA90-5E05938D5E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7457DAF0-CFD6-427C-A4BA-BD162C141835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7719,8 +7719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:OK13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="OA1" workbookViewId="0">
+      <selection activeCell="OM2" sqref="OM2:OM11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>